<commit_message>
updated diary entries for week 2
</commit_message>
<xml_diff>
--- a/diaries/diary-chunqi-zhao.xlsx
+++ b/diaries/diary-chunqi-zhao.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -74,6 +74,30 @@
   </si>
   <si>
     <t>Being able to fix build/run errors feels good.</t>
+  </si>
+  <si>
+    <t>Look at JPacMan and answer Andre's questions</t>
+  </si>
+  <si>
+    <t>Answered all questions using Ctrl+Shift+F</t>
+  </si>
+  <si>
+    <t>Being able to search through the entire project with IntelliJ is really nice</t>
+  </si>
+  <si>
+    <t>Being familiar with game dev helped a lot.</t>
+  </si>
+  <si>
+    <t>Do Pacman homework</t>
+  </si>
+  <si>
+    <t>Finished the homework and submitted pull request</t>
+  </si>
+  <si>
+    <t>Ctrl+Shift+F once again proves very useful. Creating pull request and wrestling with git on adding upstream and syncing the projects.md file took longer than the homework. Gotta sync with upstream before working on anything next time.</t>
+  </si>
+  <si>
+    <t>Frustrated with git.</t>
   </si>
 </sst>
 </file>
@@ -218,7 +242,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -264,9 +288,6 @@
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="7" fillId="4" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="7" fillId="4" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="7" fillId="4" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -628,1039 +649,1067 @@
       </c>
     </row>
     <row r="11" ht="14.25" customHeight="1">
-      <c r="A11" s="18"/>
-      <c r="B11" s="18"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="19"/>
+      <c r="A11" s="14">
+        <v>43846.0</v>
+      </c>
+      <c r="B11" s="15">
+        <v>0.75</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="F11" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="G11" s="17" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="12" ht="14.25" customHeight="1">
-      <c r="A12" s="18"/>
-      <c r="B12" s="18"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="19"/>
+      <c r="A12" s="14">
+        <v>43852.0</v>
+      </c>
+      <c r="B12" s="15">
+        <v>0.4583333333333333</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="F12" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="G12" s="17" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="13" ht="14.25" customHeight="1">
       <c r="A13" s="18"/>
-      <c r="B13" s="20"/>
-      <c r="C13" s="20"/>
-      <c r="D13" s="20"/>
-      <c r="E13" s="20"/>
-      <c r="F13" s="20"/>
-      <c r="G13" s="21"/>
+      <c r="B13" s="19"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="20"/>
     </row>
     <row r="14" ht="14.25" customHeight="1">
-      <c r="A14" s="20"/>
-      <c r="B14" s="20"/>
-      <c r="C14" s="20"/>
-      <c r="D14" s="20"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="20"/>
-      <c r="G14" s="21"/>
+      <c r="A14" s="19"/>
+      <c r="B14" s="19"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="19"/>
+      <c r="G14" s="20"/>
     </row>
     <row r="15" ht="14.25" customHeight="1">
-      <c r="A15" s="20"/>
-      <c r="B15" s="20"/>
-      <c r="C15" s="20"/>
-      <c r="D15" s="20"/>
-      <c r="E15" s="20"/>
-      <c r="F15" s="20"/>
-      <c r="G15" s="21"/>
+      <c r="A15" s="19"/>
+      <c r="B15" s="19"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="20"/>
     </row>
     <row r="16" ht="14.25" customHeight="1">
-      <c r="A16" s="20"/>
-      <c r="B16" s="20"/>
-      <c r="C16" s="20"/>
-      <c r="D16" s="20"/>
-      <c r="E16" s="20"/>
-      <c r="F16" s="20"/>
-      <c r="G16" s="21"/>
+      <c r="A16" s="19"/>
+      <c r="B16" s="19"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="20"/>
     </row>
     <row r="17" ht="14.25" customHeight="1">
       <c r="A17" s="13"/>
       <c r="B17" s="13"/>
       <c r="C17" s="13"/>
-      <c r="D17" s="20"/>
-      <c r="E17" s="20"/>
-      <c r="F17" s="20"/>
-      <c r="G17" s="21"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="19"/>
+      <c r="F17" s="19"/>
+      <c r="G17" s="20"/>
     </row>
     <row r="18" ht="14.25" customHeight="1">
-      <c r="A18" s="20"/>
-      <c r="B18" s="20"/>
-      <c r="C18" s="20"/>
+      <c r="A18" s="19"/>
+      <c r="B18" s="19"/>
+      <c r="C18" s="19"/>
       <c r="D18" s="13"/>
-      <c r="E18" s="20"/>
-      <c r="F18" s="20"/>
-      <c r="G18" s="21"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="20"/>
     </row>
     <row r="19" ht="14.25" customHeight="1">
-      <c r="A19" s="20"/>
-      <c r="B19" s="20"/>
-      <c r="C19" s="20"/>
-      <c r="D19" s="21"/>
-      <c r="E19" s="20"/>
-      <c r="F19" s="20"/>
-      <c r="G19" s="21"/>
+      <c r="A19" s="19"/>
+      <c r="B19" s="19"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="19"/>
+      <c r="F19" s="19"/>
+      <c r="G19" s="20"/>
     </row>
     <row r="20" ht="14.25" customHeight="1">
-      <c r="A20" s="20"/>
-      <c r="B20" s="20"/>
-      <c r="C20" s="20"/>
-      <c r="D20" s="21"/>
-      <c r="E20" s="20"/>
-      <c r="F20" s="20"/>
-      <c r="G20" s="21"/>
+      <c r="A20" s="19"/>
+      <c r="B20" s="19"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="19"/>
+      <c r="F20" s="19"/>
+      <c r="G20" s="20"/>
     </row>
     <row r="21" ht="14.25" customHeight="1">
-      <c r="A21" s="20"/>
-      <c r="B21" s="20"/>
-      <c r="C21" s="20"/>
-      <c r="D21" s="21"/>
-      <c r="E21" s="20"/>
-      <c r="F21" s="20"/>
-      <c r="G21" s="21"/>
+      <c r="A21" s="19"/>
+      <c r="B21" s="19"/>
+      <c r="C21" s="19"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="19"/>
+      <c r="G21" s="20"/>
     </row>
     <row r="22" ht="14.25" customHeight="1">
-      <c r="A22" s="20"/>
-      <c r="B22" s="20"/>
-      <c r="C22" s="20"/>
-      <c r="D22" s="20"/>
-      <c r="E22" s="20"/>
-      <c r="F22" s="20"/>
-      <c r="G22" s="21"/>
+      <c r="A22" s="19"/>
+      <c r="B22" s="19"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="19"/>
+      <c r="E22" s="19"/>
+      <c r="F22" s="19"/>
+      <c r="G22" s="20"/>
     </row>
     <row r="23" ht="14.25" customHeight="1">
-      <c r="A23" s="20"/>
-      <c r="B23" s="20"/>
-      <c r="C23" s="20"/>
-      <c r="D23" s="20"/>
-      <c r="E23" s="20"/>
-      <c r="F23" s="20"/>
-      <c r="G23" s="21"/>
+      <c r="A23" s="19"/>
+      <c r="B23" s="19"/>
+      <c r="C23" s="19"/>
+      <c r="D23" s="19"/>
+      <c r="E23" s="19"/>
+      <c r="F23" s="19"/>
+      <c r="G23" s="20"/>
     </row>
     <row r="24" ht="14.25" customHeight="1">
-      <c r="A24" s="20"/>
-      <c r="B24" s="20"/>
-      <c r="C24" s="20"/>
-      <c r="D24" s="20"/>
-      <c r="E24" s="20"/>
-      <c r="F24" s="20"/>
-      <c r="G24" s="21"/>
+      <c r="A24" s="19"/>
+      <c r="B24" s="19"/>
+      <c r="C24" s="19"/>
+      <c r="D24" s="19"/>
+      <c r="E24" s="19"/>
+      <c r="F24" s="19"/>
+      <c r="G24" s="20"/>
     </row>
     <row r="25" ht="14.25" customHeight="1">
-      <c r="A25" s="20"/>
-      <c r="B25" s="20"/>
-      <c r="C25" s="20"/>
-      <c r="D25" s="20"/>
-      <c r="E25" s="20"/>
-      <c r="F25" s="20"/>
-      <c r="G25" s="21"/>
+      <c r="A25" s="19"/>
+      <c r="B25" s="19"/>
+      <c r="C25" s="19"/>
+      <c r="D25" s="19"/>
+      <c r="E25" s="19"/>
+      <c r="F25" s="19"/>
+      <c r="G25" s="20"/>
     </row>
     <row r="26" ht="14.25" customHeight="1">
-      <c r="A26" s="20"/>
-      <c r="B26" s="20"/>
-      <c r="C26" s="20"/>
-      <c r="D26" s="20"/>
-      <c r="E26" s="20"/>
-      <c r="F26" s="20"/>
-      <c r="G26" s="21"/>
+      <c r="A26" s="19"/>
+      <c r="B26" s="19"/>
+      <c r="C26" s="19"/>
+      <c r="D26" s="19"/>
+      <c r="E26" s="19"/>
+      <c r="F26" s="19"/>
+      <c r="G26" s="20"/>
     </row>
     <row r="27" ht="14.25" customHeight="1">
-      <c r="A27" s="20"/>
-      <c r="B27" s="20"/>
-      <c r="C27" s="20"/>
-      <c r="D27" s="20"/>
-      <c r="E27" s="20"/>
-      <c r="F27" s="20"/>
-      <c r="G27" s="21"/>
+      <c r="A27" s="19"/>
+      <c r="B27" s="19"/>
+      <c r="C27" s="19"/>
+      <c r="D27" s="19"/>
+      <c r="E27" s="19"/>
+      <c r="F27" s="19"/>
+      <c r="G27" s="20"/>
     </row>
     <row r="28" ht="14.25" customHeight="1">
-      <c r="A28" s="20"/>
-      <c r="B28" s="20"/>
-      <c r="C28" s="20"/>
-      <c r="D28" s="20"/>
-      <c r="E28" s="20"/>
-      <c r="F28" s="20"/>
-      <c r="G28" s="21"/>
+      <c r="A28" s="19"/>
+      <c r="B28" s="19"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="20"/>
     </row>
     <row r="29" ht="14.25" customHeight="1">
-      <c r="A29" s="20"/>
-      <c r="B29" s="20"/>
-      <c r="C29" s="20"/>
-      <c r="D29" s="20"/>
-      <c r="E29" s="20"/>
-      <c r="F29" s="20"/>
-      <c r="G29" s="21"/>
+      <c r="A29" s="19"/>
+      <c r="B29" s="19"/>
+      <c r="C29" s="19"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="19"/>
+      <c r="F29" s="19"/>
+      <c r="G29" s="20"/>
     </row>
     <row r="30" ht="14.25" customHeight="1">
-      <c r="A30" s="20"/>
-      <c r="B30" s="20"/>
-      <c r="C30" s="20"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="20"/>
-      <c r="F30" s="20"/>
-      <c r="G30" s="21"/>
+      <c r="A30" s="19"/>
+      <c r="B30" s="19"/>
+      <c r="C30" s="19"/>
+      <c r="D30" s="19"/>
+      <c r="E30" s="19"/>
+      <c r="F30" s="19"/>
+      <c r="G30" s="20"/>
     </row>
     <row r="31" ht="14.25" customHeight="1">
-      <c r="A31" s="20"/>
-      <c r="B31" s="20"/>
-      <c r="C31" s="20"/>
-      <c r="D31" s="20"/>
-      <c r="E31" s="20"/>
-      <c r="F31" s="20"/>
-      <c r="G31" s="21"/>
+      <c r="A31" s="19"/>
+      <c r="B31" s="19"/>
+      <c r="C31" s="19"/>
+      <c r="D31" s="19"/>
+      <c r="E31" s="19"/>
+      <c r="F31" s="19"/>
+      <c r="G31" s="20"/>
     </row>
     <row r="32" ht="14.25" customHeight="1">
-      <c r="A32" s="20"/>
-      <c r="B32" s="20"/>
-      <c r="C32" s="20"/>
-      <c r="D32" s="20"/>
-      <c r="E32" s="20"/>
-      <c r="F32" s="20"/>
-      <c r="G32" s="21"/>
+      <c r="A32" s="19"/>
+      <c r="B32" s="19"/>
+      <c r="C32" s="19"/>
+      <c r="D32" s="19"/>
+      <c r="E32" s="19"/>
+      <c r="F32" s="19"/>
+      <c r="G32" s="20"/>
     </row>
     <row r="33" ht="14.25" customHeight="1">
-      <c r="A33" s="20"/>
-      <c r="B33" s="20"/>
-      <c r="C33" s="20"/>
-      <c r="D33" s="20"/>
-      <c r="E33" s="20"/>
-      <c r="F33" s="20"/>
-      <c r="G33" s="21"/>
+      <c r="A33" s="19"/>
+      <c r="B33" s="19"/>
+      <c r="C33" s="19"/>
+      <c r="D33" s="19"/>
+      <c r="E33" s="19"/>
+      <c r="F33" s="19"/>
+      <c r="G33" s="20"/>
     </row>
     <row r="34" ht="14.25" customHeight="1">
-      <c r="A34" s="20"/>
-      <c r="B34" s="20"/>
-      <c r="C34" s="20"/>
-      <c r="D34" s="20"/>
-      <c r="E34" s="20"/>
-      <c r="F34" s="20"/>
-      <c r="G34" s="21"/>
+      <c r="A34" s="19"/>
+      <c r="B34" s="19"/>
+      <c r="C34" s="19"/>
+      <c r="D34" s="19"/>
+      <c r="E34" s="19"/>
+      <c r="F34" s="19"/>
+      <c r="G34" s="20"/>
     </row>
     <row r="35" ht="14.25" customHeight="1">
-      <c r="A35" s="20"/>
-      <c r="B35" s="20"/>
-      <c r="C35" s="20"/>
-      <c r="D35" s="20"/>
-      <c r="E35" s="20"/>
-      <c r="F35" s="20"/>
-      <c r="G35" s="21"/>
+      <c r="A35" s="19"/>
+      <c r="B35" s="19"/>
+      <c r="C35" s="19"/>
+      <c r="D35" s="19"/>
+      <c r="E35" s="19"/>
+      <c r="F35" s="19"/>
+      <c r="G35" s="20"/>
     </row>
     <row r="36" ht="14.25" customHeight="1">
-      <c r="A36" s="20"/>
-      <c r="B36" s="20"/>
-      <c r="C36" s="20"/>
-      <c r="D36" s="20"/>
-      <c r="E36" s="20"/>
-      <c r="F36" s="20"/>
-      <c r="G36" s="21"/>
+      <c r="A36" s="19"/>
+      <c r="B36" s="19"/>
+      <c r="C36" s="19"/>
+      <c r="D36" s="19"/>
+      <c r="E36" s="19"/>
+      <c r="F36" s="19"/>
+      <c r="G36" s="20"/>
     </row>
     <row r="37" ht="14.25" customHeight="1">
-      <c r="A37" s="20"/>
-      <c r="B37" s="20"/>
-      <c r="C37" s="20"/>
-      <c r="D37" s="20"/>
-      <c r="E37" s="20"/>
-      <c r="F37" s="20"/>
-      <c r="G37" s="21"/>
+      <c r="A37" s="19"/>
+      <c r="B37" s="19"/>
+      <c r="C37" s="19"/>
+      <c r="D37" s="19"/>
+      <c r="E37" s="19"/>
+      <c r="F37" s="19"/>
+      <c r="G37" s="20"/>
     </row>
     <row r="38" ht="14.25" customHeight="1">
-      <c r="A38" s="20"/>
-      <c r="B38" s="20"/>
-      <c r="C38" s="20"/>
-      <c r="D38" s="20"/>
-      <c r="E38" s="20"/>
-      <c r="F38" s="20"/>
-      <c r="G38" s="21"/>
+      <c r="A38" s="19"/>
+      <c r="B38" s="19"/>
+      <c r="C38" s="19"/>
+      <c r="D38" s="19"/>
+      <c r="E38" s="19"/>
+      <c r="F38" s="19"/>
+      <c r="G38" s="20"/>
     </row>
     <row r="39" ht="14.25" customHeight="1">
-      <c r="A39" s="20"/>
-      <c r="B39" s="20"/>
-      <c r="C39" s="20"/>
-      <c r="D39" s="20"/>
-      <c r="E39" s="20"/>
-      <c r="F39" s="20"/>
-      <c r="G39" s="21"/>
+      <c r="A39" s="19"/>
+      <c r="B39" s="19"/>
+      <c r="C39" s="19"/>
+      <c r="D39" s="19"/>
+      <c r="E39" s="19"/>
+      <c r="F39" s="19"/>
+      <c r="G39" s="20"/>
     </row>
     <row r="40" ht="14.25" customHeight="1">
-      <c r="A40" s="20"/>
-      <c r="B40" s="20"/>
-      <c r="C40" s="20"/>
-      <c r="D40" s="20"/>
-      <c r="E40" s="20"/>
-      <c r="F40" s="20"/>
-      <c r="G40" s="21"/>
+      <c r="A40" s="19"/>
+      <c r="B40" s="19"/>
+      <c r="C40" s="19"/>
+      <c r="D40" s="19"/>
+      <c r="E40" s="19"/>
+      <c r="F40" s="19"/>
+      <c r="G40" s="20"/>
     </row>
     <row r="41" ht="14.25" customHeight="1">
-      <c r="A41" s="20"/>
-      <c r="B41" s="20"/>
-      <c r="C41" s="20"/>
-      <c r="D41" s="20"/>
-      <c r="E41" s="20"/>
-      <c r="F41" s="20"/>
-      <c r="G41" s="21"/>
+      <c r="A41" s="19"/>
+      <c r="B41" s="19"/>
+      <c r="C41" s="19"/>
+      <c r="D41" s="19"/>
+      <c r="E41" s="19"/>
+      <c r="F41" s="19"/>
+      <c r="G41" s="20"/>
     </row>
     <row r="42" ht="14.25" customHeight="1">
-      <c r="A42" s="20"/>
-      <c r="B42" s="20"/>
-      <c r="C42" s="20"/>
-      <c r="D42" s="20"/>
-      <c r="E42" s="20"/>
-      <c r="F42" s="20"/>
-      <c r="G42" s="21"/>
+      <c r="A42" s="19"/>
+      <c r="B42" s="19"/>
+      <c r="C42" s="19"/>
+      <c r="D42" s="19"/>
+      <c r="E42" s="19"/>
+      <c r="F42" s="19"/>
+      <c r="G42" s="20"/>
     </row>
     <row r="43" ht="14.25" customHeight="1">
-      <c r="A43" s="20"/>
-      <c r="B43" s="20"/>
-      <c r="C43" s="20"/>
-      <c r="D43" s="20"/>
-      <c r="E43" s="20"/>
-      <c r="F43" s="20"/>
-      <c r="G43" s="21"/>
+      <c r="A43" s="19"/>
+      <c r="B43" s="19"/>
+      <c r="C43" s="19"/>
+      <c r="D43" s="19"/>
+      <c r="E43" s="19"/>
+      <c r="F43" s="19"/>
+      <c r="G43" s="20"/>
     </row>
     <row r="44" ht="14.25" customHeight="1">
-      <c r="A44" s="20"/>
-      <c r="B44" s="20"/>
-      <c r="C44" s="20"/>
-      <c r="D44" s="20"/>
-      <c r="E44" s="20"/>
-      <c r="F44" s="20"/>
-      <c r="G44" s="21"/>
+      <c r="A44" s="19"/>
+      <c r="B44" s="19"/>
+      <c r="C44" s="19"/>
+      <c r="D44" s="19"/>
+      <c r="E44" s="19"/>
+      <c r="F44" s="19"/>
+      <c r="G44" s="20"/>
     </row>
     <row r="45" ht="14.25" customHeight="1">
-      <c r="A45" s="20"/>
-      <c r="B45" s="20"/>
-      <c r="C45" s="20"/>
-      <c r="D45" s="20"/>
-      <c r="E45" s="20"/>
-      <c r="F45" s="20"/>
-      <c r="G45" s="21"/>
+      <c r="A45" s="19"/>
+      <c r="B45" s="19"/>
+      <c r="C45" s="19"/>
+      <c r="D45" s="19"/>
+      <c r="E45" s="19"/>
+      <c r="F45" s="19"/>
+      <c r="G45" s="20"/>
     </row>
     <row r="46" ht="14.25" customHeight="1">
-      <c r="A46" s="20"/>
-      <c r="B46" s="20"/>
-      <c r="C46" s="20"/>
-      <c r="D46" s="20"/>
-      <c r="E46" s="20"/>
-      <c r="F46" s="20"/>
-      <c r="G46" s="21"/>
+      <c r="A46" s="19"/>
+      <c r="B46" s="19"/>
+      <c r="C46" s="19"/>
+      <c r="D46" s="19"/>
+      <c r="E46" s="19"/>
+      <c r="F46" s="19"/>
+      <c r="G46" s="20"/>
     </row>
     <row r="47" ht="14.25" customHeight="1">
-      <c r="A47" s="20"/>
-      <c r="B47" s="20"/>
-      <c r="C47" s="20"/>
-      <c r="D47" s="20"/>
-      <c r="E47" s="20"/>
-      <c r="F47" s="20"/>
-      <c r="G47" s="21"/>
+      <c r="A47" s="19"/>
+      <c r="B47" s="19"/>
+      <c r="C47" s="19"/>
+      <c r="D47" s="19"/>
+      <c r="E47" s="19"/>
+      <c r="F47" s="19"/>
+      <c r="G47" s="20"/>
     </row>
     <row r="48" ht="14.25" customHeight="1">
-      <c r="A48" s="20"/>
-      <c r="B48" s="20"/>
-      <c r="C48" s="20"/>
-      <c r="D48" s="20"/>
-      <c r="E48" s="20"/>
-      <c r="F48" s="20"/>
-      <c r="G48" s="21"/>
+      <c r="A48" s="19"/>
+      <c r="B48" s="19"/>
+      <c r="C48" s="19"/>
+      <c r="D48" s="19"/>
+      <c r="E48" s="19"/>
+      <c r="F48" s="19"/>
+      <c r="G48" s="20"/>
     </row>
     <row r="49" ht="14.25" customHeight="1">
-      <c r="A49" s="20"/>
-      <c r="B49" s="20"/>
-      <c r="C49" s="20"/>
-      <c r="D49" s="20"/>
-      <c r="E49" s="20"/>
-      <c r="F49" s="20"/>
-      <c r="G49" s="21"/>
+      <c r="A49" s="19"/>
+      <c r="B49" s="19"/>
+      <c r="C49" s="19"/>
+      <c r="D49" s="19"/>
+      <c r="E49" s="19"/>
+      <c r="F49" s="19"/>
+      <c r="G49" s="20"/>
     </row>
     <row r="50" ht="14.25" customHeight="1">
-      <c r="A50" s="20"/>
-      <c r="B50" s="20"/>
-      <c r="C50" s="20"/>
-      <c r="D50" s="20"/>
-      <c r="E50" s="20"/>
-      <c r="F50" s="20"/>
-      <c r="G50" s="21"/>
+      <c r="A50" s="19"/>
+      <c r="B50" s="19"/>
+      <c r="C50" s="19"/>
+      <c r="D50" s="19"/>
+      <c r="E50" s="19"/>
+      <c r="F50" s="19"/>
+      <c r="G50" s="20"/>
     </row>
     <row r="51" ht="14.25" customHeight="1">
-      <c r="A51" s="20"/>
-      <c r="B51" s="20"/>
-      <c r="C51" s="20"/>
-      <c r="D51" s="20"/>
-      <c r="E51" s="20"/>
-      <c r="F51" s="20"/>
-      <c r="G51" s="21"/>
+      <c r="A51" s="19"/>
+      <c r="B51" s="19"/>
+      <c r="C51" s="19"/>
+      <c r="D51" s="19"/>
+      <c r="E51" s="19"/>
+      <c r="F51" s="19"/>
+      <c r="G51" s="20"/>
     </row>
     <row r="52" ht="14.25" customHeight="1">
-      <c r="A52" s="20"/>
-      <c r="B52" s="20"/>
-      <c r="C52" s="20"/>
-      <c r="D52" s="20"/>
-      <c r="E52" s="20"/>
-      <c r="F52" s="20"/>
-      <c r="G52" s="21"/>
+      <c r="A52" s="19"/>
+      <c r="B52" s="19"/>
+      <c r="C52" s="19"/>
+      <c r="D52" s="19"/>
+      <c r="E52" s="19"/>
+      <c r="F52" s="19"/>
+      <c r="G52" s="20"/>
     </row>
     <row r="53" ht="14.25" customHeight="1">
-      <c r="A53" s="20"/>
-      <c r="B53" s="20"/>
-      <c r="C53" s="20"/>
-      <c r="D53" s="20"/>
-      <c r="E53" s="20"/>
-      <c r="F53" s="20"/>
-      <c r="G53" s="21"/>
+      <c r="A53" s="19"/>
+      <c r="B53" s="19"/>
+      <c r="C53" s="19"/>
+      <c r="D53" s="19"/>
+      <c r="E53" s="19"/>
+      <c r="F53" s="19"/>
+      <c r="G53" s="20"/>
     </row>
     <row r="54" ht="14.25" customHeight="1">
-      <c r="A54" s="20"/>
-      <c r="B54" s="20"/>
-      <c r="C54" s="20"/>
-      <c r="D54" s="20"/>
-      <c r="E54" s="20"/>
-      <c r="F54" s="20"/>
-      <c r="G54" s="21"/>
+      <c r="A54" s="19"/>
+      <c r="B54" s="19"/>
+      <c r="C54" s="19"/>
+      <c r="D54" s="19"/>
+      <c r="E54" s="19"/>
+      <c r="F54" s="19"/>
+      <c r="G54" s="20"/>
     </row>
     <row r="55" ht="14.25" customHeight="1">
-      <c r="A55" s="20"/>
-      <c r="B55" s="20"/>
-      <c r="C55" s="20"/>
-      <c r="D55" s="20"/>
-      <c r="E55" s="20"/>
-      <c r="F55" s="20"/>
-      <c r="G55" s="21"/>
+      <c r="A55" s="19"/>
+      <c r="B55" s="19"/>
+      <c r="C55" s="19"/>
+      <c r="D55" s="19"/>
+      <c r="E55" s="19"/>
+      <c r="F55" s="19"/>
+      <c r="G55" s="20"/>
     </row>
     <row r="56" ht="14.25" customHeight="1">
-      <c r="A56" s="20"/>
-      <c r="B56" s="20"/>
-      <c r="C56" s="20"/>
-      <c r="D56" s="20"/>
-      <c r="E56" s="20"/>
-      <c r="F56" s="20"/>
-      <c r="G56" s="21"/>
+      <c r="A56" s="19"/>
+      <c r="B56" s="19"/>
+      <c r="C56" s="19"/>
+      <c r="D56" s="19"/>
+      <c r="E56" s="19"/>
+      <c r="F56" s="19"/>
+      <c r="G56" s="20"/>
     </row>
     <row r="57" ht="14.25" customHeight="1">
-      <c r="A57" s="20"/>
-      <c r="B57" s="20"/>
-      <c r="C57" s="20"/>
-      <c r="D57" s="20"/>
-      <c r="E57" s="20"/>
-      <c r="F57" s="20"/>
-      <c r="G57" s="21"/>
+      <c r="A57" s="19"/>
+      <c r="B57" s="19"/>
+      <c r="C57" s="19"/>
+      <c r="D57" s="19"/>
+      <c r="E57" s="19"/>
+      <c r="F57" s="19"/>
+      <c r="G57" s="20"/>
     </row>
     <row r="58" ht="14.25" customHeight="1">
-      <c r="A58" s="20"/>
-      <c r="B58" s="20"/>
-      <c r="C58" s="20"/>
-      <c r="D58" s="20"/>
-      <c r="E58" s="20"/>
-      <c r="F58" s="20"/>
-      <c r="G58" s="21"/>
+      <c r="A58" s="19"/>
+      <c r="B58" s="19"/>
+      <c r="C58" s="19"/>
+      <c r="D58" s="19"/>
+      <c r="E58" s="19"/>
+      <c r="F58" s="19"/>
+      <c r="G58" s="20"/>
     </row>
     <row r="59" ht="14.25" customHeight="1">
-      <c r="A59" s="20"/>
-      <c r="B59" s="20"/>
-      <c r="C59" s="20"/>
-      <c r="D59" s="20"/>
-      <c r="E59" s="20"/>
-      <c r="F59" s="20"/>
-      <c r="G59" s="21"/>
+      <c r="A59" s="19"/>
+      <c r="B59" s="19"/>
+      <c r="C59" s="19"/>
+      <c r="D59" s="19"/>
+      <c r="E59" s="19"/>
+      <c r="F59" s="19"/>
+      <c r="G59" s="20"/>
     </row>
     <row r="60" ht="14.25" customHeight="1">
-      <c r="A60" s="20"/>
-      <c r="B60" s="20"/>
-      <c r="C60" s="20"/>
-      <c r="D60" s="20"/>
-      <c r="E60" s="20"/>
-      <c r="F60" s="20"/>
-      <c r="G60" s="21"/>
+      <c r="A60" s="19"/>
+      <c r="B60" s="19"/>
+      <c r="C60" s="19"/>
+      <c r="D60" s="19"/>
+      <c r="E60" s="19"/>
+      <c r="F60" s="19"/>
+      <c r="G60" s="20"/>
     </row>
     <row r="61" ht="14.25" customHeight="1">
-      <c r="A61" s="20"/>
-      <c r="B61" s="20"/>
-      <c r="C61" s="20"/>
-      <c r="D61" s="20"/>
-      <c r="E61" s="20"/>
-      <c r="F61" s="20"/>
-      <c r="G61" s="21"/>
+      <c r="A61" s="19"/>
+      <c r="B61" s="19"/>
+      <c r="C61" s="19"/>
+      <c r="D61" s="19"/>
+      <c r="E61" s="19"/>
+      <c r="F61" s="19"/>
+      <c r="G61" s="20"/>
     </row>
     <row r="62" ht="14.25" customHeight="1">
-      <c r="A62" s="20"/>
-      <c r="B62" s="20"/>
-      <c r="C62" s="20"/>
-      <c r="D62" s="20"/>
-      <c r="E62" s="20"/>
-      <c r="F62" s="20"/>
-      <c r="G62" s="21"/>
+      <c r="A62" s="19"/>
+      <c r="B62" s="19"/>
+      <c r="C62" s="19"/>
+      <c r="D62" s="19"/>
+      <c r="E62" s="19"/>
+      <c r="F62" s="19"/>
+      <c r="G62" s="20"/>
     </row>
     <row r="63" ht="14.25" customHeight="1">
-      <c r="A63" s="20"/>
-      <c r="B63" s="20"/>
-      <c r="C63" s="20"/>
-      <c r="D63" s="20"/>
-      <c r="E63" s="20"/>
-      <c r="F63" s="20"/>
-      <c r="G63" s="21"/>
+      <c r="A63" s="19"/>
+      <c r="B63" s="19"/>
+      <c r="C63" s="19"/>
+      <c r="D63" s="19"/>
+      <c r="E63" s="19"/>
+      <c r="F63" s="19"/>
+      <c r="G63" s="20"/>
     </row>
     <row r="64" ht="14.25" customHeight="1">
-      <c r="A64" s="20"/>
-      <c r="B64" s="20"/>
-      <c r="C64" s="20"/>
-      <c r="D64" s="20"/>
-      <c r="E64" s="20"/>
-      <c r="F64" s="20"/>
-      <c r="G64" s="21"/>
+      <c r="A64" s="19"/>
+      <c r="B64" s="19"/>
+      <c r="C64" s="19"/>
+      <c r="D64" s="19"/>
+      <c r="E64" s="19"/>
+      <c r="F64" s="19"/>
+      <c r="G64" s="20"/>
     </row>
     <row r="65" ht="14.25" customHeight="1">
-      <c r="A65" s="20"/>
-      <c r="B65" s="20"/>
-      <c r="C65" s="20"/>
-      <c r="D65" s="20"/>
-      <c r="E65" s="20"/>
-      <c r="F65" s="20"/>
-      <c r="G65" s="21"/>
+      <c r="A65" s="19"/>
+      <c r="B65" s="19"/>
+      <c r="C65" s="19"/>
+      <c r="D65" s="19"/>
+      <c r="E65" s="19"/>
+      <c r="F65" s="19"/>
+      <c r="G65" s="20"/>
     </row>
     <row r="66" ht="14.25" customHeight="1">
-      <c r="A66" s="20"/>
-      <c r="B66" s="20"/>
-      <c r="C66" s="20"/>
-      <c r="D66" s="20"/>
-      <c r="E66" s="20"/>
-      <c r="F66" s="20"/>
-      <c r="G66" s="21"/>
+      <c r="A66" s="19"/>
+      <c r="B66" s="19"/>
+      <c r="C66" s="19"/>
+      <c r="D66" s="19"/>
+      <c r="E66" s="19"/>
+      <c r="F66" s="19"/>
+      <c r="G66" s="20"/>
     </row>
     <row r="67" ht="14.25" customHeight="1">
-      <c r="A67" s="20"/>
-      <c r="B67" s="20"/>
-      <c r="C67" s="20"/>
-      <c r="D67" s="20"/>
-      <c r="E67" s="20"/>
-      <c r="F67" s="20"/>
-      <c r="G67" s="21"/>
+      <c r="A67" s="19"/>
+      <c r="B67" s="19"/>
+      <c r="C67" s="19"/>
+      <c r="D67" s="19"/>
+      <c r="E67" s="19"/>
+      <c r="F67" s="19"/>
+      <c r="G67" s="20"/>
     </row>
     <row r="68" ht="14.25" customHeight="1">
-      <c r="A68" s="20"/>
-      <c r="B68" s="20"/>
-      <c r="C68" s="20"/>
-      <c r="D68" s="20"/>
-      <c r="E68" s="20"/>
-      <c r="F68" s="20"/>
-      <c r="G68" s="21"/>
+      <c r="A68" s="19"/>
+      <c r="B68" s="19"/>
+      <c r="C68" s="19"/>
+      <c r="D68" s="19"/>
+      <c r="E68" s="19"/>
+      <c r="F68" s="19"/>
+      <c r="G68" s="20"/>
     </row>
     <row r="69" ht="14.25" customHeight="1">
-      <c r="A69" s="20"/>
-      <c r="B69" s="20"/>
-      <c r="C69" s="20"/>
-      <c r="D69" s="20"/>
-      <c r="E69" s="20"/>
-      <c r="F69" s="20"/>
-      <c r="G69" s="21"/>
+      <c r="A69" s="19"/>
+      <c r="B69" s="19"/>
+      <c r="C69" s="19"/>
+      <c r="D69" s="19"/>
+      <c r="E69" s="19"/>
+      <c r="F69" s="19"/>
+      <c r="G69" s="20"/>
     </row>
     <row r="70" ht="14.25" customHeight="1">
-      <c r="A70" s="20"/>
-      <c r="B70" s="20"/>
-      <c r="C70" s="20"/>
-      <c r="D70" s="20"/>
-      <c r="E70" s="20"/>
-      <c r="F70" s="20"/>
-      <c r="G70" s="21"/>
+      <c r="A70" s="19"/>
+      <c r="B70" s="19"/>
+      <c r="C70" s="19"/>
+      <c r="D70" s="19"/>
+      <c r="E70" s="19"/>
+      <c r="F70" s="19"/>
+      <c r="G70" s="20"/>
     </row>
     <row r="71" ht="14.25" customHeight="1">
-      <c r="A71" s="20"/>
-      <c r="B71" s="20"/>
-      <c r="C71" s="20"/>
-      <c r="D71" s="20"/>
-      <c r="E71" s="20"/>
-      <c r="F71" s="20"/>
-      <c r="G71" s="21"/>
+      <c r="A71" s="19"/>
+      <c r="B71" s="19"/>
+      <c r="C71" s="19"/>
+      <c r="D71" s="19"/>
+      <c r="E71" s="19"/>
+      <c r="F71" s="19"/>
+      <c r="G71" s="20"/>
     </row>
     <row r="72" ht="14.25" customHeight="1">
-      <c r="A72" s="20"/>
-      <c r="B72" s="20"/>
-      <c r="C72" s="20"/>
-      <c r="D72" s="20"/>
-      <c r="E72" s="20"/>
-      <c r="F72" s="20"/>
-      <c r="G72" s="21"/>
+      <c r="A72" s="19"/>
+      <c r="B72" s="19"/>
+      <c r="C72" s="19"/>
+      <c r="D72" s="19"/>
+      <c r="E72" s="19"/>
+      <c r="F72" s="19"/>
+      <c r="G72" s="20"/>
     </row>
     <row r="73" ht="14.25" customHeight="1">
-      <c r="A73" s="20"/>
-      <c r="B73" s="20"/>
-      <c r="C73" s="20"/>
-      <c r="D73" s="20"/>
-      <c r="E73" s="20"/>
-      <c r="F73" s="20"/>
-      <c r="G73" s="21"/>
+      <c r="A73" s="19"/>
+      <c r="B73" s="19"/>
+      <c r="C73" s="19"/>
+      <c r="D73" s="19"/>
+      <c r="E73" s="19"/>
+      <c r="F73" s="19"/>
+      <c r="G73" s="20"/>
     </row>
     <row r="74" ht="14.25" customHeight="1">
-      <c r="A74" s="20"/>
-      <c r="B74" s="20"/>
-      <c r="C74" s="20"/>
-      <c r="D74" s="20"/>
-      <c r="E74" s="20"/>
-      <c r="F74" s="20"/>
-      <c r="G74" s="21"/>
+      <c r="A74" s="19"/>
+      <c r="B74" s="19"/>
+      <c r="C74" s="19"/>
+      <c r="D74" s="19"/>
+      <c r="E74" s="19"/>
+      <c r="F74" s="19"/>
+      <c r="G74" s="20"/>
     </row>
     <row r="75" ht="14.25" customHeight="1">
-      <c r="A75" s="20"/>
-      <c r="B75" s="20"/>
-      <c r="C75" s="20"/>
-      <c r="D75" s="20"/>
-      <c r="E75" s="20"/>
-      <c r="F75" s="20"/>
-      <c r="G75" s="21"/>
+      <c r="A75" s="19"/>
+      <c r="B75" s="19"/>
+      <c r="C75" s="19"/>
+      <c r="D75" s="19"/>
+      <c r="E75" s="19"/>
+      <c r="F75" s="19"/>
+      <c r="G75" s="20"/>
     </row>
     <row r="76" ht="14.25" customHeight="1">
-      <c r="A76" s="20"/>
-      <c r="B76" s="20"/>
-      <c r="C76" s="20"/>
-      <c r="D76" s="20"/>
-      <c r="E76" s="20"/>
-      <c r="F76" s="20"/>
-      <c r="G76" s="21"/>
+      <c r="A76" s="19"/>
+      <c r="B76" s="19"/>
+      <c r="C76" s="19"/>
+      <c r="D76" s="19"/>
+      <c r="E76" s="19"/>
+      <c r="F76" s="19"/>
+      <c r="G76" s="20"/>
     </row>
     <row r="77" ht="14.25" customHeight="1">
-      <c r="A77" s="20"/>
-      <c r="B77" s="20"/>
-      <c r="C77" s="20"/>
-      <c r="D77" s="20"/>
-      <c r="E77" s="20"/>
-      <c r="F77" s="20"/>
-      <c r="G77" s="21"/>
+      <c r="A77" s="19"/>
+      <c r="B77" s="19"/>
+      <c r="C77" s="19"/>
+      <c r="D77" s="19"/>
+      <c r="E77" s="19"/>
+      <c r="F77" s="19"/>
+      <c r="G77" s="20"/>
     </row>
     <row r="78" ht="14.25" customHeight="1">
-      <c r="A78" s="20"/>
-      <c r="B78" s="20"/>
-      <c r="C78" s="20"/>
-      <c r="D78" s="20"/>
-      <c r="E78" s="20"/>
-      <c r="F78" s="20"/>
-      <c r="G78" s="21"/>
+      <c r="A78" s="19"/>
+      <c r="B78" s="19"/>
+      <c r="C78" s="19"/>
+      <c r="D78" s="19"/>
+      <c r="E78" s="19"/>
+      <c r="F78" s="19"/>
+      <c r="G78" s="20"/>
     </row>
     <row r="79" ht="14.25" customHeight="1">
-      <c r="A79" s="20"/>
-      <c r="B79" s="20"/>
-      <c r="C79" s="20"/>
-      <c r="D79" s="20"/>
-      <c r="E79" s="20"/>
-      <c r="F79" s="20"/>
-      <c r="G79" s="21"/>
+      <c r="A79" s="19"/>
+      <c r="B79" s="19"/>
+      <c r="C79" s="19"/>
+      <c r="D79" s="19"/>
+      <c r="E79" s="19"/>
+      <c r="F79" s="19"/>
+      <c r="G79" s="20"/>
     </row>
     <row r="80" ht="14.25" customHeight="1">
-      <c r="A80" s="20"/>
-      <c r="B80" s="20"/>
-      <c r="C80" s="20"/>
-      <c r="D80" s="20"/>
-      <c r="E80" s="20"/>
-      <c r="F80" s="20"/>
-      <c r="G80" s="21"/>
+      <c r="A80" s="19"/>
+      <c r="B80" s="19"/>
+      <c r="C80" s="19"/>
+      <c r="D80" s="19"/>
+      <c r="E80" s="19"/>
+      <c r="F80" s="19"/>
+      <c r="G80" s="20"/>
     </row>
     <row r="81" ht="14.25" customHeight="1">
-      <c r="A81" s="20"/>
-      <c r="B81" s="20"/>
-      <c r="C81" s="20"/>
-      <c r="D81" s="20"/>
-      <c r="E81" s="20"/>
-      <c r="F81" s="20"/>
-      <c r="G81" s="21"/>
+      <c r="A81" s="19"/>
+      <c r="B81" s="19"/>
+      <c r="C81" s="19"/>
+      <c r="D81" s="19"/>
+      <c r="E81" s="19"/>
+      <c r="F81" s="19"/>
+      <c r="G81" s="20"/>
     </row>
     <row r="82" ht="14.25" customHeight="1">
-      <c r="A82" s="20"/>
-      <c r="B82" s="20"/>
-      <c r="C82" s="20"/>
-      <c r="D82" s="20"/>
-      <c r="E82" s="20"/>
-      <c r="F82" s="20"/>
-      <c r="G82" s="21"/>
+      <c r="A82" s="19"/>
+      <c r="B82" s="19"/>
+      <c r="C82" s="19"/>
+      <c r="D82" s="19"/>
+      <c r="E82" s="19"/>
+      <c r="F82" s="19"/>
+      <c r="G82" s="20"/>
     </row>
     <row r="83" ht="14.25" customHeight="1">
-      <c r="A83" s="20"/>
-      <c r="B83" s="20"/>
-      <c r="C83" s="20"/>
-      <c r="D83" s="20"/>
-      <c r="E83" s="20"/>
-      <c r="F83" s="20"/>
-      <c r="G83" s="21"/>
+      <c r="A83" s="19"/>
+      <c r="B83" s="19"/>
+      <c r="C83" s="19"/>
+      <c r="D83" s="19"/>
+      <c r="E83" s="19"/>
+      <c r="F83" s="19"/>
+      <c r="G83" s="20"/>
     </row>
     <row r="84" ht="14.25" customHeight="1">
-      <c r="A84" s="20"/>
-      <c r="B84" s="20"/>
-      <c r="C84" s="20"/>
-      <c r="D84" s="20"/>
-      <c r="E84" s="20"/>
-      <c r="F84" s="20"/>
-      <c r="G84" s="21"/>
+      <c r="A84" s="19"/>
+      <c r="B84" s="19"/>
+      <c r="C84" s="19"/>
+      <c r="D84" s="19"/>
+      <c r="E84" s="19"/>
+      <c r="F84" s="19"/>
+      <c r="G84" s="20"/>
     </row>
     <row r="85" ht="14.25" customHeight="1">
-      <c r="A85" s="20"/>
-      <c r="B85" s="20"/>
-      <c r="C85" s="20"/>
-      <c r="D85" s="20"/>
-      <c r="E85" s="20"/>
-      <c r="F85" s="20"/>
-      <c r="G85" s="21"/>
+      <c r="A85" s="19"/>
+      <c r="B85" s="19"/>
+      <c r="C85" s="19"/>
+      <c r="D85" s="19"/>
+      <c r="E85" s="19"/>
+      <c r="F85" s="19"/>
+      <c r="G85" s="20"/>
     </row>
     <row r="86" ht="14.25" customHeight="1">
-      <c r="A86" s="20"/>
-      <c r="B86" s="20"/>
-      <c r="C86" s="20"/>
-      <c r="D86" s="20"/>
-      <c r="E86" s="20"/>
-      <c r="F86" s="20"/>
-      <c r="G86" s="21"/>
+      <c r="A86" s="19"/>
+      <c r="B86" s="19"/>
+      <c r="C86" s="19"/>
+      <c r="D86" s="19"/>
+      <c r="E86" s="19"/>
+      <c r="F86" s="19"/>
+      <c r="G86" s="20"/>
     </row>
     <row r="87" ht="14.25" customHeight="1">
-      <c r="A87" s="20"/>
-      <c r="B87" s="20"/>
-      <c r="C87" s="20"/>
-      <c r="D87" s="20"/>
-      <c r="E87" s="20"/>
-      <c r="F87" s="20"/>
-      <c r="G87" s="21"/>
+      <c r="A87" s="19"/>
+      <c r="B87" s="19"/>
+      <c r="C87" s="19"/>
+      <c r="D87" s="19"/>
+      <c r="E87" s="19"/>
+      <c r="F87" s="19"/>
+      <c r="G87" s="20"/>
     </row>
     <row r="88" ht="14.25" customHeight="1">
-      <c r="A88" s="20"/>
-      <c r="B88" s="20"/>
-      <c r="C88" s="20"/>
-      <c r="D88" s="20"/>
-      <c r="E88" s="20"/>
-      <c r="F88" s="20"/>
-      <c r="G88" s="21"/>
+      <c r="A88" s="19"/>
+      <c r="B88" s="19"/>
+      <c r="C88" s="19"/>
+      <c r="D88" s="19"/>
+      <c r="E88" s="19"/>
+      <c r="F88" s="19"/>
+      <c r="G88" s="20"/>
     </row>
     <row r="89" ht="14.25" customHeight="1">
-      <c r="A89" s="20"/>
-      <c r="B89" s="20"/>
-      <c r="C89" s="20"/>
-      <c r="D89" s="20"/>
-      <c r="E89" s="20"/>
-      <c r="F89" s="20"/>
-      <c r="G89" s="21"/>
+      <c r="A89" s="19"/>
+      <c r="B89" s="19"/>
+      <c r="C89" s="19"/>
+      <c r="D89" s="19"/>
+      <c r="E89" s="19"/>
+      <c r="F89" s="19"/>
+      <c r="G89" s="20"/>
     </row>
     <row r="90" ht="14.25" customHeight="1">
-      <c r="A90" s="20"/>
-      <c r="B90" s="20"/>
-      <c r="C90" s="20"/>
-      <c r="D90" s="20"/>
-      <c r="E90" s="20"/>
-      <c r="F90" s="20"/>
-      <c r="G90" s="21"/>
+      <c r="A90" s="19"/>
+      <c r="B90" s="19"/>
+      <c r="C90" s="19"/>
+      <c r="D90" s="19"/>
+      <c r="E90" s="19"/>
+      <c r="F90" s="19"/>
+      <c r="G90" s="20"/>
     </row>
     <row r="91" ht="14.25" customHeight="1">
-      <c r="A91" s="20"/>
-      <c r="B91" s="20"/>
-      <c r="C91" s="20"/>
-      <c r="D91" s="20"/>
-      <c r="E91" s="20"/>
-      <c r="F91" s="20"/>
-      <c r="G91" s="21"/>
+      <c r="A91" s="19"/>
+      <c r="B91" s="19"/>
+      <c r="C91" s="19"/>
+      <c r="D91" s="19"/>
+      <c r="E91" s="19"/>
+      <c r="F91" s="19"/>
+      <c r="G91" s="20"/>
     </row>
     <row r="92" ht="14.25" customHeight="1">
-      <c r="A92" s="20"/>
-      <c r="B92" s="20"/>
-      <c r="C92" s="20"/>
-      <c r="D92" s="20"/>
-      <c r="E92" s="20"/>
-      <c r="F92" s="20"/>
-      <c r="G92" s="21"/>
+      <c r="A92" s="19"/>
+      <c r="B92" s="19"/>
+      <c r="C92" s="19"/>
+      <c r="D92" s="19"/>
+      <c r="E92" s="19"/>
+      <c r="F92" s="19"/>
+      <c r="G92" s="20"/>
     </row>
     <row r="93" ht="14.25" customHeight="1">
-      <c r="A93" s="20"/>
-      <c r="B93" s="20"/>
-      <c r="C93" s="20"/>
-      <c r="D93" s="20"/>
-      <c r="E93" s="20"/>
-      <c r="F93" s="20"/>
-      <c r="G93" s="21"/>
+      <c r="A93" s="19"/>
+      <c r="B93" s="19"/>
+      <c r="C93" s="19"/>
+      <c r="D93" s="19"/>
+      <c r="E93" s="19"/>
+      <c r="F93" s="19"/>
+      <c r="G93" s="20"/>
     </row>
     <row r="94" ht="14.25" customHeight="1">
-      <c r="A94" s="20"/>
-      <c r="B94" s="20"/>
-      <c r="C94" s="20"/>
-      <c r="D94" s="20"/>
-      <c r="E94" s="20"/>
-      <c r="F94" s="20"/>
-      <c r="G94" s="21"/>
+      <c r="A94" s="19"/>
+      <c r="B94" s="19"/>
+      <c r="C94" s="19"/>
+      <c r="D94" s="19"/>
+      <c r="E94" s="19"/>
+      <c r="F94" s="19"/>
+      <c r="G94" s="20"/>
     </row>
     <row r="95" ht="14.25" customHeight="1">
-      <c r="A95" s="20"/>
-      <c r="B95" s="20"/>
-      <c r="C95" s="20"/>
-      <c r="D95" s="20"/>
-      <c r="E95" s="20"/>
-      <c r="F95" s="20"/>
-      <c r="G95" s="21"/>
+      <c r="A95" s="19"/>
+      <c r="B95" s="19"/>
+      <c r="C95" s="19"/>
+      <c r="D95" s="19"/>
+      <c r="E95" s="19"/>
+      <c r="F95" s="19"/>
+      <c r="G95" s="20"/>
     </row>
     <row r="96" ht="14.25" customHeight="1">
-      <c r="A96" s="20"/>
-      <c r="B96" s="20"/>
-      <c r="C96" s="20"/>
-      <c r="D96" s="20"/>
-      <c r="E96" s="20"/>
-      <c r="F96" s="20"/>
-      <c r="G96" s="21"/>
+      <c r="A96" s="19"/>
+      <c r="B96" s="19"/>
+      <c r="C96" s="19"/>
+      <c r="D96" s="19"/>
+      <c r="E96" s="19"/>
+      <c r="F96" s="19"/>
+      <c r="G96" s="20"/>
     </row>
     <row r="97" ht="14.25" customHeight="1">
-      <c r="A97" s="20"/>
-      <c r="B97" s="20"/>
-      <c r="C97" s="20"/>
-      <c r="D97" s="20"/>
-      <c r="E97" s="20"/>
-      <c r="F97" s="20"/>
-      <c r="G97" s="21"/>
+      <c r="A97" s="19"/>
+      <c r="B97" s="19"/>
+      <c r="C97" s="19"/>
+      <c r="D97" s="19"/>
+      <c r="E97" s="19"/>
+      <c r="F97" s="19"/>
+      <c r="G97" s="20"/>
     </row>
     <row r="98" ht="14.25" customHeight="1">
-      <c r="A98" s="20"/>
-      <c r="B98" s="20"/>
-      <c r="C98" s="20"/>
-      <c r="D98" s="20"/>
-      <c r="E98" s="20"/>
-      <c r="F98" s="20"/>
-      <c r="G98" s="21"/>
+      <c r="A98" s="19"/>
+      <c r="B98" s="19"/>
+      <c r="C98" s="19"/>
+      <c r="D98" s="19"/>
+      <c r="E98" s="19"/>
+      <c r="F98" s="19"/>
+      <c r="G98" s="20"/>
     </row>
     <row r="99" ht="14.25" customHeight="1">
-      <c r="A99" s="20"/>
-      <c r="B99" s="20"/>
-      <c r="C99" s="20"/>
-      <c r="D99" s="20"/>
-      <c r="E99" s="20"/>
-      <c r="F99" s="20"/>
-      <c r="G99" s="21"/>
+      <c r="A99" s="19"/>
+      <c r="B99" s="19"/>
+      <c r="C99" s="19"/>
+      <c r="D99" s="19"/>
+      <c r="E99" s="19"/>
+      <c r="F99" s="19"/>
+      <c r="G99" s="20"/>
     </row>
     <row r="100" ht="14.25" customHeight="1">
-      <c r="A100" s="20"/>
-      <c r="B100" s="20"/>
-      <c r="C100" s="20"/>
-      <c r="D100" s="20"/>
-      <c r="E100" s="20"/>
-      <c r="F100" s="20"/>
-      <c r="G100" s="21"/>
+      <c r="A100" s="19"/>
+      <c r="B100" s="19"/>
+      <c r="C100" s="19"/>
+      <c r="D100" s="19"/>
+      <c r="E100" s="19"/>
+      <c r="F100" s="19"/>
+      <c r="G100" s="20"/>
     </row>
     <row r="101" ht="14.25" customHeight="1">
-      <c r="A101" s="20"/>
-      <c r="B101" s="20"/>
-      <c r="C101" s="20"/>
-      <c r="D101" s="20"/>
-      <c r="E101" s="20"/>
-      <c r="F101" s="20"/>
-      <c r="G101" s="21"/>
+      <c r="A101" s="19"/>
+      <c r="B101" s="19"/>
+      <c r="C101" s="19"/>
+      <c r="D101" s="19"/>
+      <c r="E101" s="19"/>
+      <c r="F101" s="19"/>
+      <c r="G101" s="20"/>
     </row>
     <row r="102" ht="14.25" customHeight="1">
-      <c r="A102" s="20"/>
-      <c r="B102" s="20"/>
-      <c r="C102" s="20"/>
-      <c r="D102" s="20"/>
-      <c r="E102" s="20"/>
-      <c r="F102" s="20"/>
-      <c r="G102" s="21"/>
+      <c r="A102" s="19"/>
+      <c r="B102" s="19"/>
+      <c r="C102" s="19"/>
+      <c r="D102" s="19"/>
+      <c r="E102" s="19"/>
+      <c r="F102" s="19"/>
+      <c r="G102" s="20"/>
     </row>
     <row r="103" ht="14.25" customHeight="1">
-      <c r="A103" s="20"/>
-      <c r="B103" s="20"/>
-      <c r="C103" s="20"/>
-      <c r="D103" s="20"/>
-      <c r="E103" s="20"/>
-      <c r="F103" s="20"/>
-      <c r="G103" s="21"/>
+      <c r="A103" s="19"/>
+      <c r="B103" s="19"/>
+      <c r="C103" s="19"/>
+      <c r="D103" s="19"/>
+      <c r="E103" s="19"/>
+      <c r="F103" s="19"/>
+      <c r="G103" s="20"/>
     </row>
     <row r="104" ht="14.25" customHeight="1">
-      <c r="A104" s="20"/>
-      <c r="B104" s="20"/>
-      <c r="C104" s="20"/>
-      <c r="D104" s="20"/>
-      <c r="E104" s="20"/>
-      <c r="F104" s="20"/>
-      <c r="G104" s="21"/>
+      <c r="A104" s="19"/>
+      <c r="B104" s="19"/>
+      <c r="C104" s="19"/>
+      <c r="D104" s="19"/>
+      <c r="E104" s="19"/>
+      <c r="F104" s="19"/>
+      <c r="G104" s="20"/>
     </row>
     <row r="105" ht="14.25" customHeight="1">
-      <c r="A105" s="20"/>
-      <c r="B105" s="20"/>
-      <c r="C105" s="20"/>
-      <c r="D105" s="20"/>
-      <c r="E105" s="20"/>
-      <c r="F105" s="20"/>
-      <c r="G105" s="21"/>
+      <c r="A105" s="19"/>
+      <c r="B105" s="19"/>
+      <c r="C105" s="19"/>
+      <c r="D105" s="19"/>
+      <c r="E105" s="19"/>
+      <c r="F105" s="19"/>
+      <c r="G105" s="20"/>
     </row>
     <row r="106" ht="14.25" customHeight="1">
-      <c r="A106" s="20"/>
-      <c r="B106" s="20"/>
-      <c r="C106" s="20"/>
-      <c r="D106" s="20"/>
-      <c r="E106" s="20"/>
-      <c r="F106" s="20"/>
-      <c r="G106" s="21"/>
+      <c r="A106" s="19"/>
+      <c r="B106" s="19"/>
+      <c r="C106" s="19"/>
+      <c r="D106" s="19"/>
+      <c r="E106" s="19"/>
+      <c r="F106" s="19"/>
+      <c r="G106" s="20"/>
     </row>
     <row r="107" ht="14.25" customHeight="1">
-      <c r="A107" s="20"/>
-      <c r="B107" s="20"/>
-      <c r="C107" s="20"/>
-      <c r="D107" s="20"/>
-      <c r="E107" s="20"/>
-      <c r="F107" s="20"/>
-      <c r="G107" s="21"/>
+      <c r="A107" s="19"/>
+      <c r="B107" s="19"/>
+      <c r="C107" s="19"/>
+      <c r="D107" s="19"/>
+      <c r="E107" s="19"/>
+      <c r="F107" s="19"/>
+      <c r="G107" s="20"/>
     </row>
     <row r="108" ht="14.25" customHeight="1">
-      <c r="A108" s="20"/>
-      <c r="B108" s="20"/>
-      <c r="C108" s="20"/>
-      <c r="D108" s="20"/>
-      <c r="E108" s="20"/>
-      <c r="F108" s="20"/>
-      <c r="G108" s="21"/>
+      <c r="A108" s="19"/>
+      <c r="B108" s="19"/>
+      <c r="C108" s="19"/>
+      <c r="D108" s="19"/>
+      <c r="E108" s="19"/>
+      <c r="F108" s="19"/>
+      <c r="G108" s="20"/>
     </row>
     <row r="109" ht="14.25" customHeight="1">
-      <c r="A109" s="20"/>
-      <c r="B109" s="20"/>
-      <c r="C109" s="20"/>
-      <c r="D109" s="20"/>
-      <c r="E109" s="20"/>
-      <c r="F109" s="20"/>
-      <c r="G109" s="21"/>
+      <c r="A109" s="19"/>
+      <c r="B109" s="19"/>
+      <c r="C109" s="19"/>
+      <c r="D109" s="19"/>
+      <c r="E109" s="19"/>
+      <c r="F109" s="19"/>
+      <c r="G109" s="20"/>
     </row>
     <row r="110" ht="14.25" customHeight="1">
-      <c r="A110" s="20"/>
-      <c r="B110" s="20"/>
-      <c r="C110" s="20"/>
-      <c r="D110" s="20"/>
-      <c r="E110" s="20"/>
-      <c r="F110" s="20"/>
-      <c r="G110" s="21"/>
+      <c r="A110" s="19"/>
+      <c r="B110" s="19"/>
+      <c r="C110" s="19"/>
+      <c r="D110" s="19"/>
+      <c r="E110" s="19"/>
+      <c r="F110" s="19"/>
+      <c r="G110" s="20"/>
     </row>
     <row r="111" ht="14.25" customHeight="1">
-      <c r="A111" s="20"/>
-      <c r="B111" s="20"/>
-      <c r="C111" s="20"/>
-      <c r="D111" s="20"/>
-      <c r="E111" s="20"/>
-      <c r="F111" s="20"/>
-      <c r="G111" s="21"/>
+      <c r="A111" s="19"/>
+      <c r="B111" s="19"/>
+      <c r="C111" s="19"/>
+      <c r="D111" s="19"/>
+      <c r="E111" s="19"/>
+      <c r="F111" s="19"/>
+      <c r="G111" s="20"/>
     </row>
     <row r="112" ht="14.25" customHeight="1">
-      <c r="A112" s="20"/>
-      <c r="B112" s="20"/>
-      <c r="C112" s="20"/>
-      <c r="D112" s="20"/>
-      <c r="E112" s="20"/>
-      <c r="F112" s="20"/>
-      <c r="G112" s="21"/>
+      <c r="A112" s="19"/>
+      <c r="B112" s="19"/>
+      <c r="C112" s="19"/>
+      <c r="D112" s="19"/>
+      <c r="E112" s="19"/>
+      <c r="F112" s="19"/>
+      <c r="G112" s="20"/>
     </row>
     <row r="113" ht="14.25" customHeight="1">
-      <c r="A113" s="20"/>
-      <c r="B113" s="20"/>
-      <c r="C113" s="20"/>
-      <c r="D113" s="20"/>
-      <c r="E113" s="20"/>
-      <c r="F113" s="20"/>
-      <c r="G113" s="21"/>
+      <c r="A113" s="19"/>
+      <c r="B113" s="19"/>
+      <c r="C113" s="19"/>
+      <c r="D113" s="19"/>
+      <c r="E113" s="19"/>
+      <c r="F113" s="19"/>
+      <c r="G113" s="20"/>
     </row>
     <row r="114" ht="14.25" customHeight="1">
-      <c r="A114" s="20"/>
-      <c r="B114" s="20"/>
-      <c r="C114" s="20"/>
-      <c r="D114" s="20"/>
-      <c r="E114" s="20"/>
-      <c r="F114" s="20"/>
-      <c r="G114" s="21"/>
+      <c r="A114" s="19"/>
+      <c r="B114" s="19"/>
+      <c r="C114" s="19"/>
+      <c r="D114" s="19"/>
+      <c r="E114" s="19"/>
+      <c r="F114" s="19"/>
+      <c r="G114" s="20"/>
     </row>
     <row r="115" ht="14.25" customHeight="1">
-      <c r="A115" s="20"/>
-      <c r="B115" s="20"/>
-      <c r="C115" s="20"/>
-      <c r="D115" s="20"/>
-      <c r="E115" s="20"/>
-      <c r="F115" s="20"/>
-      <c r="G115" s="21"/>
+      <c r="A115" s="19"/>
+      <c r="B115" s="19"/>
+      <c r="C115" s="19"/>
+      <c r="D115" s="19"/>
+      <c r="E115" s="19"/>
+      <c r="F115" s="19"/>
+      <c r="G115" s="20"/>
     </row>
     <row r="116" ht="14.25" customHeight="1">
-      <c r="A116" s="20"/>
-      <c r="B116" s="20"/>
-      <c r="C116" s="20"/>
-      <c r="D116" s="20"/>
-      <c r="E116" s="20"/>
-      <c r="F116" s="20"/>
-      <c r="G116" s="21"/>
+      <c r="A116" s="19"/>
+      <c r="B116" s="19"/>
+      <c r="C116" s="19"/>
+      <c r="D116" s="19"/>
+      <c r="E116" s="19"/>
+      <c r="F116" s="19"/>
+      <c r="G116" s="20"/>
     </row>
     <row r="117" ht="14.25" customHeight="1">
-      <c r="A117" s="20"/>
-      <c r="B117" s="20"/>
-      <c r="C117" s="20"/>
-      <c r="D117" s="20"/>
-      <c r="E117" s="20"/>
-      <c r="F117" s="20"/>
-      <c r="G117" s="21"/>
+      <c r="A117" s="19"/>
+      <c r="B117" s="19"/>
+      <c r="C117" s="19"/>
+      <c r="D117" s="19"/>
+      <c r="E117" s="19"/>
+      <c r="F117" s="19"/>
+      <c r="G117" s="20"/>
     </row>
     <row r="118" ht="14.25" customHeight="1">
-      <c r="A118" s="20"/>
-      <c r="B118" s="20"/>
-      <c r="C118" s="20"/>
-      <c r="D118" s="20"/>
-      <c r="E118" s="20"/>
-      <c r="F118" s="20"/>
-      <c r="G118" s="21"/>
+      <c r="A118" s="19"/>
+      <c r="B118" s="19"/>
+      <c r="C118" s="19"/>
+      <c r="D118" s="19"/>
+      <c r="E118" s="19"/>
+      <c r="F118" s="19"/>
+      <c r="G118" s="20"/>
     </row>
     <row r="119" ht="14.25" customHeight="1">
-      <c r="A119" s="20"/>
-      <c r="B119" s="20"/>
-      <c r="C119" s="20"/>
-      <c r="D119" s="20"/>
-      <c r="E119" s="20"/>
-      <c r="F119" s="20"/>
-      <c r="G119" s="21"/>
+      <c r="A119" s="19"/>
+      <c r="B119" s="19"/>
+      <c r="C119" s="19"/>
+      <c r="D119" s="19"/>
+      <c r="E119" s="19"/>
+      <c r="F119" s="19"/>
+      <c r="G119" s="20"/>
     </row>
     <row r="120" ht="14.25" customHeight="1">
-      <c r="A120" s="20"/>
-      <c r="B120" s="20"/>
-      <c r="C120" s="20"/>
-      <c r="D120" s="20"/>
-      <c r="E120" s="20"/>
-      <c r="F120" s="20"/>
-      <c r="G120" s="21"/>
+      <c r="A120" s="19"/>
+      <c r="B120" s="19"/>
+      <c r="C120" s="19"/>
+      <c r="D120" s="19"/>
+      <c r="E120" s="19"/>
+      <c r="F120" s="19"/>
+      <c r="G120" s="20"/>
     </row>
     <row r="121" ht="14.25" customHeight="1">
-      <c r="A121" s="20"/>
-      <c r="B121" s="20"/>
-      <c r="C121" s="20"/>
-      <c r="D121" s="20"/>
-      <c r="E121" s="20"/>
-      <c r="F121" s="20"/>
-      <c r="G121" s="21"/>
+      <c r="A121" s="19"/>
+      <c r="B121" s="19"/>
+      <c r="C121" s="19"/>
+      <c r="D121" s="19"/>
+      <c r="E121" s="19"/>
+      <c r="F121" s="19"/>
+      <c r="G121" s="20"/>
     </row>
     <row r="122" ht="14.25" customHeight="1">
-      <c r="A122" s="20"/>
-      <c r="B122" s="20"/>
-      <c r="C122" s="20"/>
-      <c r="D122" s="20"/>
-      <c r="E122" s="20"/>
-      <c r="F122" s="20"/>
-      <c r="G122" s="21"/>
+      <c r="A122" s="19"/>
+      <c r="B122" s="19"/>
+      <c r="C122" s="19"/>
+      <c r="D122" s="19"/>
+      <c r="E122" s="19"/>
+      <c r="F122" s="19"/>
+      <c r="G122" s="20"/>
     </row>
     <row r="123" ht="14.25" customHeight="1">
-      <c r="A123" s="20"/>
-      <c r="B123" s="20"/>
-      <c r="C123" s="20"/>
-      <c r="D123" s="20"/>
-      <c r="E123" s="20"/>
-      <c r="F123" s="20"/>
-      <c r="G123" s="21"/>
+      <c r="A123" s="19"/>
+      <c r="B123" s="19"/>
+      <c r="C123" s="19"/>
+      <c r="D123" s="19"/>
+      <c r="E123" s="19"/>
+      <c r="F123" s="19"/>
+      <c r="G123" s="20"/>
     </row>
     <row r="124" ht="14.25" customHeight="1">
-      <c r="A124" s="20"/>
-      <c r="B124" s="20"/>
-      <c r="C124" s="20"/>
-      <c r="D124" s="20"/>
-      <c r="E124" s="20"/>
-      <c r="F124" s="20"/>
-      <c r="G124" s="21"/>
+      <c r="A124" s="19"/>
+      <c r="B124" s="19"/>
+      <c r="C124" s="19"/>
+      <c r="D124" s="19"/>
+      <c r="E124" s="19"/>
+      <c r="F124" s="19"/>
+      <c r="G124" s="20"/>
     </row>
     <row r="125" ht="14.25" customHeight="1">
-      <c r="A125" s="20"/>
-      <c r="B125" s="20"/>
-      <c r="C125" s="20"/>
-      <c r="D125" s="20"/>
-      <c r="E125" s="20"/>
-      <c r="F125" s="20"/>
-      <c r="G125" s="21"/>
+      <c r="A125" s="19"/>
+      <c r="B125" s="19"/>
+      <c r="C125" s="19"/>
+      <c r="D125" s="19"/>
+      <c r="E125" s="19"/>
+      <c r="F125" s="19"/>
+      <c r="G125" s="20"/>
     </row>
     <row r="126" ht="14.25" customHeight="1"/>
     <row r="127" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
updated diary for week 3
</commit_message>
<xml_diff>
--- a/diaries/diary-chunqi-zhao.xlsx
+++ b/diaries/diary-chunqi-zhao.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="49">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -98,6 +98,72 @@
   </si>
   <si>
     <t>Frustrated with git.</t>
+  </si>
+  <si>
+    <t>Harry</t>
+  </si>
+  <si>
+    <t>Create UML diagram for Pacman</t>
+  </si>
+  <si>
+    <t>UML Digram created with SimpleUMLCE</t>
+  </si>
+  <si>
+    <t>Quite simple to do, the tool is very easy to use, automatic layout is nice</t>
+  </si>
+  <si>
+    <t>Pretty good.</t>
+  </si>
+  <si>
+    <t>Print out UML diagram for Runelite</t>
+  </si>
+  <si>
+    <t>Exported as png file full resolution, sliced into 10 by 10 images with GIMP, and Printed 21 images that were relevant</t>
+  </si>
+  <si>
+    <t>Figuring out how to cut the image using gimp was a process in itself. The image being 33771 x 25215 pixels didn't help. A lot of trees were wasted today.</t>
+  </si>
+  <si>
+    <t>Learning how to use gimp felt good.</t>
+  </si>
+  <si>
+    <t>Stich up the printed UML diagram for Runelite</t>
+  </si>
+  <si>
+    <t>Pieced together the UML diagram with tape</t>
+  </si>
+  <si>
+    <t>Huge PITA.</t>
+  </si>
+  <si>
+    <t>Frustrated.</t>
+  </si>
+  <si>
+    <t>Thuc, Harry</t>
+  </si>
+  <si>
+    <t>Figure out what features to do with the team</t>
+  </si>
+  <si>
+    <t>Choose Screenmarkers and metronome plugins</t>
+  </si>
+  <si>
+    <t>Metronome plugin was fairly straight forward, screenmarkers was decently challenging</t>
+  </si>
+  <si>
+    <t>Good.</t>
+  </si>
+  <si>
+    <t>Final check on writeup, highlight on printed UML diagram</t>
+  </si>
+  <si>
+    <t>Cleaned up writeup and Harry submitted pull request, Thuc and I went over UML diagram and highlighted relevant parts to screenmarkers and metronome</t>
+  </si>
+  <si>
+    <t>Trying to find something on the UML diagram was a huge PITA, since its barely readable.</t>
+  </si>
+  <si>
+    <t>Good, since its finally over.</t>
   </si>
 </sst>
 </file>
@@ -108,7 +174,7 @@
     <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
     <numFmt numFmtId="165" formatCode="h:mm am/pm"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="15">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -167,6 +233,11 @@
     <font>
       <i/>
       <sz val="11.0"/>
+      <color rgb="FF006100"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12.0"/>
       <color rgb="FF006100"/>
     </font>
     <font>
@@ -287,13 +358,13 @@
     <xf borderId="7" fillId="4" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="7" fillId="4" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="7" fillId="4" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="7" fillId="4" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="7" fillId="4" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="7" fillId="4" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="7" fillId="4" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -695,44 +766,100 @@
       </c>
     </row>
     <row r="13" ht="14.25" customHeight="1">
-      <c r="A13" s="18"/>
-      <c r="B13" s="19"/>
-      <c r="C13" s="19"/>
-      <c r="D13" s="19"/>
-      <c r="E13" s="19"/>
-      <c r="F13" s="19"/>
-      <c r="G13" s="20"/>
+      <c r="A13" s="14">
+        <v>43853.0</v>
+      </c>
+      <c r="B13" s="15">
+        <v>0.75</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="E13" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="F13" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="G13" s="17" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="14" ht="14.25" customHeight="1">
-      <c r="A14" s="19"/>
-      <c r="B14" s="19"/>
-      <c r="C14" s="19"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="19"/>
-      <c r="F14" s="19"/>
-      <c r="G14" s="20"/>
+      <c r="A14" s="14">
+        <v>43857.0</v>
+      </c>
+      <c r="B14" s="15">
+        <v>0.8333333333333334</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="E14" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="F14" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="G14" s="17" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="15" ht="14.25" customHeight="1">
-      <c r="A15" s="19"/>
-      <c r="B15" s="19"/>
-      <c r="C15" s="19"/>
-      <c r="D15" s="19"/>
-      <c r="E15" s="19"/>
-      <c r="F15" s="19"/>
-      <c r="G15" s="20"/>
+      <c r="A15" s="14">
+        <v>43859.0</v>
+      </c>
+      <c r="B15" s="15">
+        <v>0.5416666666666666</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="E15" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="F15" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="G15" s="17" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="16" ht="14.25" customHeight="1">
-      <c r="A16" s="19"/>
-      <c r="B16" s="19"/>
-      <c r="C16" s="19"/>
-      <c r="D16" s="19"/>
-      <c r="E16" s="19"/>
-      <c r="F16" s="19"/>
-      <c r="G16" s="20"/>
+      <c r="A16" s="14">
+        <v>43859.0</v>
+      </c>
+      <c r="B16" s="15">
+        <v>0.6458333333333334</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="D16" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="E16" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="F16" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="G16" s="17" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="17" ht="14.25" customHeight="1">
-      <c r="A17" s="13"/>
-      <c r="B17" s="13"/>
+      <c r="A17" s="18"/>
+      <c r="B17" s="18"/>
       <c r="C17" s="13"/>
       <c r="D17" s="19"/>
       <c r="E17" s="19"/>
@@ -749,13 +876,27 @@
       <c r="G18" s="20"/>
     </row>
     <row r="19" ht="14.25" customHeight="1">
-      <c r="A19" s="19"/>
-      <c r="B19" s="19"/>
-      <c r="C19" s="19"/>
-      <c r="D19" s="20"/>
-      <c r="E19" s="19"/>
-      <c r="F19" s="19"/>
-      <c r="G19" s="20"/>
+      <c r="A19" s="14">
+        <v>43860.0</v>
+      </c>
+      <c r="B19" s="15">
+        <v>0.6458333333333334</v>
+      </c>
+      <c r="C19" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="D19" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="E19" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="F19" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="G19" s="17" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="20" ht="14.25" customHeight="1">
       <c r="A20" s="19"/>

</xml_diff>

<commit_message>
updated diary for week 4
</commit_message>
<xml_diff>
--- a/diaries/diary-chunqi-zhao.xlsx
+++ b/diaries/diary-chunqi-zhao.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="65">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -164,6 +164,54 @@
   </si>
   <si>
     <t>Good, since its finally over.</t>
+  </si>
+  <si>
+    <t>Learn how to generate call graphs and sequence diagrams with IntelliJ on Pacman</t>
+  </si>
+  <si>
+    <t>Was able to generate call graphs and sequence diagrams</t>
+  </si>
+  <si>
+    <t>The call graphs seem very useful and intuitive looking, sequence diagrams not so much</t>
+  </si>
+  <si>
+    <t>Learning new things always good.</t>
+  </si>
+  <si>
+    <t>Choose 2 essential features on Runelite for write up</t>
+  </si>
+  <si>
+    <t>Found the plugin manager feature to be very essential to the client, also chose the idlenotifier plugin as it is very essential to the player</t>
+  </si>
+  <si>
+    <t>Apparently everything relevant in runelite is coded as a plugin. So it ended up being pretty hard to find another essential client feature, so we decided to find a feature that was essential to the players instead</t>
+  </si>
+  <si>
+    <t>Tired, worked on both writeups up till very late.</t>
+  </si>
+  <si>
+    <t>Edit and print the graphs and diagrams</t>
+  </si>
+  <si>
+    <t>Printed each on one piece of paper this time, everything still visible</t>
+  </si>
+  <si>
+    <t>Call graphs plugin on IntelliJ does not have a export feature, which is very annoying as I had to screen shot the diagram with a vertical ultrawide monitor</t>
+  </si>
+  <si>
+    <t>Could be worse.</t>
+  </si>
+  <si>
+    <t>Final check on writeup, push required files to repo</t>
+  </si>
+  <si>
+    <t>pull request submitted</t>
+  </si>
+  <si>
+    <t>Nothing much to reflect on</t>
+  </si>
+  <si>
+    <t>Good, ready for class.</t>
   </si>
 </sst>
 </file>
@@ -174,7 +222,7 @@
     <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
     <numFmt numFmtId="165" formatCode="h:mm am/pm"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="12">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -191,12 +239,10 @@
       <b/>
       <sz val="12.0"/>
       <color rgb="FF9C5700"/>
-      <name val="Calibri"/>
     </font>
     <font>
       <sz val="11.0"/>
       <color rgb="FF9C5700"/>
-      <name val="Calibri"/>
     </font>
     <font>
       <i/>
@@ -212,26 +258,8 @@
     <font>
       <sz val="12.0"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
     </font>
     <font>
-      <sz val="11.0"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12.0"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="12.0"/>
-      <color rgb="FF006100"/>
-    </font>
-    <font>
-      <i/>
       <sz val="11.0"/>
       <color rgb="FF006100"/>
     </font>
@@ -244,13 +272,11 @@
       <i/>
       <sz val="12.0"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
     </font>
     <font>
       <i/>
       <sz val="11.0"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="5">
@@ -279,41 +305,90 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="11">
     <border/>
     <border>
-      <left/>
-      <top/>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
     </border>
     <border>
-      <top/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
     </border>
     <border>
-      <right/>
-      <top/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
     </border>
     <border>
-      <left/>
-      <bottom/>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
     </border>
     <border>
-      <bottom/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
     </border>
     <border>
-      <right/>
-      <bottom/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="24">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -328,43 +403,52 @@
     <xf borderId="7" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="7" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="7" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="8" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="7" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="7" fillId="4" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="4" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="7" fillId="4" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="5" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="7" fillId="4" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="6" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="9" fillId="4" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="9" fillId="4" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="10" fillId="4" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="7" fillId="4" fontId="10" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="10" fillId="4" fontId="10" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="7" fillId="4" fontId="10" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="10" fillId="4" fontId="10" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="7" fillId="4" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="10" fillId="4" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="7" fillId="4" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="10" fillId="4" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="7" fillId="4" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="7" fillId="4" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="10" fillId="4" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="7" fillId="4" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="10" fillId="4" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -576,10 +660,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
-    <pageSetUpPr/>
+    <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="9.0" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="B11" sqref="B11" pane="bottomLeft"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
@@ -609,1249 +696,481 @@
     </row>
     <row r="3" ht="14.25" customHeight="1">
       <c r="A3" s="7"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="8"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="9"/>
     </row>
     <row r="4" ht="14.25" customHeight="1">
       <c r="A4" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="9"/>
     </row>
     <row r="5" ht="14.25" customHeight="1">
       <c r="A5" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="9"/>
     </row>
     <row r="6" ht="14.25" customHeight="1">
       <c r="A6" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="9"/>
     </row>
     <row r="7" ht="14.25" customHeight="1">
-      <c r="A7" s="7"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="8"/>
+      <c r="A7" s="12"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="14"/>
     </row>
     <row r="8" ht="14.25" customHeight="1">
-      <c r="A8" s="11"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="12"/>
+      <c r="A8" s="15"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="16"/>
     </row>
     <row r="9" ht="14.25" customHeight="1">
-      <c r="A9" s="13" t="s">
+      <c r="A9" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="D9" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="13" t="s">
+      <c r="E9" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="13" t="s">
+      <c r="F9" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="G9" s="13" t="s">
+      <c r="G9" s="17" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="10" ht="14.25" customHeight="1">
-      <c r="A10" s="14">
+      <c r="A10" s="18">
         <v>43839.0</v>
       </c>
-      <c r="B10" s="15">
+      <c r="B10" s="19">
         <v>0.7916666666666666</v>
       </c>
-      <c r="C10" s="16" t="s">
+      <c r="C10" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="16" t="s">
+      <c r="D10" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="16" t="s">
+      <c r="E10" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="F10" s="16" t="s">
+      <c r="F10" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="G10" s="17" t="s">
+      <c r="G10" s="21" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="11" ht="14.25" customHeight="1">
-      <c r="A11" s="14">
+      <c r="A11" s="18">
         <v>43846.0</v>
       </c>
-      <c r="B11" s="15">
+      <c r="B11" s="19">
         <v>0.75</v>
       </c>
-      <c r="C11" s="16" t="s">
+      <c r="C11" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="16" t="s">
+      <c r="D11" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="E11" s="16" t="s">
+      <c r="E11" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="F11" s="16" t="s">
+      <c r="F11" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="G11" s="17" t="s">
+      <c r="G11" s="21" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="12" ht="14.25" customHeight="1">
-      <c r="A12" s="14">
+      <c r="A12" s="18">
         <v>43852.0</v>
       </c>
-      <c r="B12" s="15">
+      <c r="B12" s="19">
         <v>0.4583333333333333</v>
       </c>
-      <c r="C12" s="16" t="s">
+      <c r="C12" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="D12" s="16" t="s">
+      <c r="D12" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="E12" s="16" t="s">
+      <c r="E12" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="F12" s="16" t="s">
+      <c r="F12" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="G12" s="17" t="s">
+      <c r="G12" s="21" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="13" ht="14.25" customHeight="1">
-      <c r="A13" s="14">
+      <c r="A13" s="18">
         <v>43853.0</v>
       </c>
-      <c r="B13" s="15">
+      <c r="B13" s="19">
         <v>0.75</v>
       </c>
-      <c r="C13" s="16" t="s">
+      <c r="C13" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="D13" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="E13" s="16" t="s">
+      <c r="E13" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="F13" s="16" t="s">
+      <c r="F13" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="G13" s="17" t="s">
+      <c r="G13" s="21" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="14" ht="14.25" customHeight="1">
-      <c r="A14" s="14">
+      <c r="A14" s="18">
         <v>43857.0</v>
       </c>
-      <c r="B14" s="15">
+      <c r="B14" s="19">
         <v>0.8333333333333334</v>
       </c>
-      <c r="C14" s="16" t="s">
+      <c r="C14" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="16" t="s">
+      <c r="D14" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="E14" s="16" t="s">
+      <c r="E14" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="F14" s="16" t="s">
+      <c r="F14" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="G14" s="17" t="s">
+      <c r="G14" s="21" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="15" ht="14.25" customHeight="1">
-      <c r="A15" s="14">
+      <c r="A15" s="18">
         <v>43859.0</v>
       </c>
-      <c r="B15" s="15">
+      <c r="B15" s="19">
         <v>0.5416666666666666</v>
       </c>
-      <c r="C15" s="16" t="s">
+      <c r="C15" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="16" t="s">
+      <c r="D15" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="E15" s="16" t="s">
+      <c r="E15" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="F15" s="16" t="s">
+      <c r="F15" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="G15" s="17" t="s">
+      <c r="G15" s="21" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="16" ht="14.25" customHeight="1">
-      <c r="A16" s="14">
+      <c r="A16" s="18">
         <v>43859.0</v>
       </c>
-      <c r="B16" s="15">
+      <c r="B16" s="19">
         <v>0.6458333333333334</v>
       </c>
-      <c r="C16" s="16" t="s">
+      <c r="C16" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="D16" s="16" t="s">
+      <c r="D16" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="E16" s="16" t="s">
+      <c r="E16" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="F16" s="16" t="s">
+      <c r="F16" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="G16" s="17" t="s">
+      <c r="G16" s="21" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="17" ht="14.25" customHeight="1">
-      <c r="A17" s="18"/>
-      <c r="B17" s="18"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="19"/>
-      <c r="E17" s="19"/>
-      <c r="F17" s="19"/>
-      <c r="G17" s="20"/>
+      <c r="A17" s="18">
+        <v>43860.0</v>
+      </c>
+      <c r="B17" s="19">
+        <v>0.6458333333333334</v>
+      </c>
+      <c r="C17" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="E17" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="F17" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="G17" s="21" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="18" ht="14.25" customHeight="1">
-      <c r="A18" s="19"/>
-      <c r="B18" s="19"/>
-      <c r="C18" s="19"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="19"/>
-      <c r="F18" s="19"/>
-      <c r="G18" s="20"/>
+      <c r="A18" s="18">
+        <v>43860.0</v>
+      </c>
+      <c r="B18" s="19">
+        <v>0.75</v>
+      </c>
+      <c r="C18" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="E18" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="F18" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="G18" s="21" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="19" ht="14.25" customHeight="1">
-      <c r="A19" s="14">
-        <v>43860.0</v>
-      </c>
-      <c r="B19" s="15">
-        <v>0.6458333333333334</v>
-      </c>
-      <c r="C19" s="16" t="s">
+      <c r="A19" s="18">
+        <v>43866.0</v>
+      </c>
+      <c r="B19" s="19">
+        <v>0.8333333333333334</v>
+      </c>
+      <c r="C19" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="D19" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="E19" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="F19" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="G19" s="17" t="s">
-        <v>48</v>
+      <c r="D19" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="E19" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="F19" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="G19" s="21" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="20" ht="14.25" customHeight="1">
-      <c r="A20" s="19"/>
-      <c r="B20" s="19"/>
-      <c r="C20" s="19"/>
-      <c r="D20" s="20"/>
-      <c r="E20" s="19"/>
-      <c r="F20" s="19"/>
-      <c r="G20" s="20"/>
+      <c r="A20" s="18">
+        <v>43867.0</v>
+      </c>
+      <c r="B20" s="19">
+        <v>0.5416666666666666</v>
+      </c>
+      <c r="C20" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D20" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="E20" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="F20" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="G20" s="21" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="21" ht="14.25" customHeight="1">
-      <c r="A21" s="19"/>
-      <c r="B21" s="19"/>
-      <c r="C21" s="19"/>
-      <c r="D21" s="20"/>
-      <c r="E21" s="19"/>
-      <c r="F21" s="19"/>
-      <c r="G21" s="20"/>
+      <c r="A21" s="18">
+        <v>43867.0</v>
+      </c>
+      <c r="B21" s="19">
+        <v>0.6666666666666666</v>
+      </c>
+      <c r="C21" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="D21" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="E21" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="F21" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="G21" s="21" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="22" ht="14.25" customHeight="1">
-      <c r="A22" s="19"/>
-      <c r="B22" s="19"/>
-      <c r="C22" s="19"/>
-      <c r="D22" s="19"/>
-      <c r="E22" s="19"/>
-      <c r="F22" s="19"/>
-      <c r="G22" s="20"/>
-    </row>
-    <row r="23" ht="14.25" customHeight="1">
-      <c r="A23" s="19"/>
-      <c r="B23" s="19"/>
-      <c r="C23" s="19"/>
-      <c r="D23" s="19"/>
-      <c r="E23" s="19"/>
-      <c r="F23" s="19"/>
-      <c r="G23" s="20"/>
-    </row>
-    <row r="24" ht="14.25" customHeight="1">
-      <c r="A24" s="19"/>
-      <c r="B24" s="19"/>
-      <c r="C24" s="19"/>
-      <c r="D24" s="19"/>
-      <c r="E24" s="19"/>
-      <c r="F24" s="19"/>
-      <c r="G24" s="20"/>
-    </row>
-    <row r="25" ht="14.25" customHeight="1">
-      <c r="A25" s="19"/>
-      <c r="B25" s="19"/>
-      <c r="C25" s="19"/>
-      <c r="D25" s="19"/>
-      <c r="E25" s="19"/>
-      <c r="F25" s="19"/>
-      <c r="G25" s="20"/>
-    </row>
-    <row r="26" ht="14.25" customHeight="1">
-      <c r="A26" s="19"/>
-      <c r="B26" s="19"/>
-      <c r="C26" s="19"/>
-      <c r="D26" s="19"/>
-      <c r="E26" s="19"/>
-      <c r="F26" s="19"/>
-      <c r="G26" s="20"/>
-    </row>
-    <row r="27" ht="14.25" customHeight="1">
-      <c r="A27" s="19"/>
-      <c r="B27" s="19"/>
-      <c r="C27" s="19"/>
-      <c r="D27" s="19"/>
-      <c r="E27" s="19"/>
-      <c r="F27" s="19"/>
-      <c r="G27" s="20"/>
-    </row>
-    <row r="28" ht="14.25" customHeight="1">
-      <c r="A28" s="19"/>
-      <c r="B28" s="19"/>
-      <c r="C28" s="19"/>
-      <c r="D28" s="19"/>
-      <c r="E28" s="19"/>
-      <c r="F28" s="19"/>
-      <c r="G28" s="20"/>
-    </row>
-    <row r="29" ht="14.25" customHeight="1">
-      <c r="A29" s="19"/>
-      <c r="B29" s="19"/>
-      <c r="C29" s="19"/>
-      <c r="D29" s="19"/>
-      <c r="E29" s="19"/>
-      <c r="F29" s="19"/>
-      <c r="G29" s="20"/>
-    </row>
-    <row r="30" ht="14.25" customHeight="1">
-      <c r="A30" s="19"/>
-      <c r="B30" s="19"/>
-      <c r="C30" s="19"/>
-      <c r="D30" s="19"/>
-      <c r="E30" s="19"/>
-      <c r="F30" s="19"/>
-      <c r="G30" s="20"/>
-    </row>
-    <row r="31" ht="14.25" customHeight="1">
-      <c r="A31" s="19"/>
-      <c r="B31" s="19"/>
-      <c r="C31" s="19"/>
-      <c r="D31" s="19"/>
-      <c r="E31" s="19"/>
-      <c r="F31" s="19"/>
-      <c r="G31" s="20"/>
-    </row>
-    <row r="32" ht="14.25" customHeight="1">
-      <c r="A32" s="19"/>
-      <c r="B32" s="19"/>
-      <c r="C32" s="19"/>
-      <c r="D32" s="19"/>
-      <c r="E32" s="19"/>
-      <c r="F32" s="19"/>
-      <c r="G32" s="20"/>
-    </row>
-    <row r="33" ht="14.25" customHeight="1">
-      <c r="A33" s="19"/>
-      <c r="B33" s="19"/>
-      <c r="C33" s="19"/>
-      <c r="D33" s="19"/>
-      <c r="E33" s="19"/>
-      <c r="F33" s="19"/>
-      <c r="G33" s="20"/>
-    </row>
-    <row r="34" ht="14.25" customHeight="1">
-      <c r="A34" s="19"/>
-      <c r="B34" s="19"/>
-      <c r="C34" s="19"/>
-      <c r="D34" s="19"/>
-      <c r="E34" s="19"/>
-      <c r="F34" s="19"/>
-      <c r="G34" s="20"/>
-    </row>
-    <row r="35" ht="14.25" customHeight="1">
-      <c r="A35" s="19"/>
-      <c r="B35" s="19"/>
-      <c r="C35" s="19"/>
-      <c r="D35" s="19"/>
-      <c r="E35" s="19"/>
-      <c r="F35" s="19"/>
-      <c r="G35" s="20"/>
-    </row>
-    <row r="36" ht="14.25" customHeight="1">
-      <c r="A36" s="19"/>
-      <c r="B36" s="19"/>
-      <c r="C36" s="19"/>
-      <c r="D36" s="19"/>
-      <c r="E36" s="19"/>
-      <c r="F36" s="19"/>
-      <c r="G36" s="20"/>
-    </row>
-    <row r="37" ht="14.25" customHeight="1">
-      <c r="A37" s="19"/>
-      <c r="B37" s="19"/>
-      <c r="C37" s="19"/>
-      <c r="D37" s="19"/>
-      <c r="E37" s="19"/>
-      <c r="F37" s="19"/>
-      <c r="G37" s="20"/>
-    </row>
-    <row r="38" ht="14.25" customHeight="1">
-      <c r="A38" s="19"/>
-      <c r="B38" s="19"/>
-      <c r="C38" s="19"/>
-      <c r="D38" s="19"/>
-      <c r="E38" s="19"/>
-      <c r="F38" s="19"/>
-      <c r="G38" s="20"/>
-    </row>
-    <row r="39" ht="14.25" customHeight="1">
-      <c r="A39" s="19"/>
-      <c r="B39" s="19"/>
-      <c r="C39" s="19"/>
-      <c r="D39" s="19"/>
-      <c r="E39" s="19"/>
-      <c r="F39" s="19"/>
-      <c r="G39" s="20"/>
-    </row>
-    <row r="40" ht="14.25" customHeight="1">
-      <c r="A40" s="19"/>
-      <c r="B40" s="19"/>
-      <c r="C40" s="19"/>
-      <c r="D40" s="19"/>
-      <c r="E40" s="19"/>
-      <c r="F40" s="19"/>
-      <c r="G40" s="20"/>
-    </row>
-    <row r="41" ht="14.25" customHeight="1">
-      <c r="A41" s="19"/>
-      <c r="B41" s="19"/>
-      <c r="C41" s="19"/>
-      <c r="D41" s="19"/>
-      <c r="E41" s="19"/>
-      <c r="F41" s="19"/>
-      <c r="G41" s="20"/>
-    </row>
-    <row r="42" ht="14.25" customHeight="1">
-      <c r="A42" s="19"/>
-      <c r="B42" s="19"/>
-      <c r="C42" s="19"/>
-      <c r="D42" s="19"/>
-      <c r="E42" s="19"/>
-      <c r="F42" s="19"/>
-      <c r="G42" s="20"/>
-    </row>
-    <row r="43" ht="14.25" customHeight="1">
-      <c r="A43" s="19"/>
-      <c r="B43" s="19"/>
-      <c r="C43" s="19"/>
-      <c r="D43" s="19"/>
-      <c r="E43" s="19"/>
-      <c r="F43" s="19"/>
-      <c r="G43" s="20"/>
-    </row>
-    <row r="44" ht="14.25" customHeight="1">
-      <c r="A44" s="19"/>
-      <c r="B44" s="19"/>
-      <c r="C44" s="19"/>
-      <c r="D44" s="19"/>
-      <c r="E44" s="19"/>
-      <c r="F44" s="19"/>
-      <c r="G44" s="20"/>
-    </row>
-    <row r="45" ht="14.25" customHeight="1">
-      <c r="A45" s="19"/>
-      <c r="B45" s="19"/>
-      <c r="C45" s="19"/>
-      <c r="D45" s="19"/>
-      <c r="E45" s="19"/>
-      <c r="F45" s="19"/>
-      <c r="G45" s="20"/>
-    </row>
-    <row r="46" ht="14.25" customHeight="1">
-      <c r="A46" s="19"/>
-      <c r="B46" s="19"/>
-      <c r="C46" s="19"/>
-      <c r="D46" s="19"/>
-      <c r="E46" s="19"/>
-      <c r="F46" s="19"/>
-      <c r="G46" s="20"/>
-    </row>
-    <row r="47" ht="14.25" customHeight="1">
-      <c r="A47" s="19"/>
-      <c r="B47" s="19"/>
-      <c r="C47" s="19"/>
-      <c r="D47" s="19"/>
-      <c r="E47" s="19"/>
-      <c r="F47" s="19"/>
-      <c r="G47" s="20"/>
-    </row>
-    <row r="48" ht="14.25" customHeight="1">
-      <c r="A48" s="19"/>
-      <c r="B48" s="19"/>
-      <c r="C48" s="19"/>
-      <c r="D48" s="19"/>
-      <c r="E48" s="19"/>
-      <c r="F48" s="19"/>
-      <c r="G48" s="20"/>
-    </row>
-    <row r="49" ht="14.25" customHeight="1">
-      <c r="A49" s="19"/>
-      <c r="B49" s="19"/>
-      <c r="C49" s="19"/>
-      <c r="D49" s="19"/>
-      <c r="E49" s="19"/>
-      <c r="F49" s="19"/>
-      <c r="G49" s="20"/>
-    </row>
-    <row r="50" ht="14.25" customHeight="1">
-      <c r="A50" s="19"/>
-      <c r="B50" s="19"/>
-      <c r="C50" s="19"/>
-      <c r="D50" s="19"/>
-      <c r="E50" s="19"/>
-      <c r="F50" s="19"/>
-      <c r="G50" s="20"/>
-    </row>
-    <row r="51" ht="14.25" customHeight="1">
-      <c r="A51" s="19"/>
-      <c r="B51" s="19"/>
-      <c r="C51" s="19"/>
-      <c r="D51" s="19"/>
-      <c r="E51" s="19"/>
-      <c r="F51" s="19"/>
-      <c r="G51" s="20"/>
-    </row>
-    <row r="52" ht="14.25" customHeight="1">
-      <c r="A52" s="19"/>
-      <c r="B52" s="19"/>
-      <c r="C52" s="19"/>
-      <c r="D52" s="19"/>
-      <c r="E52" s="19"/>
-      <c r="F52" s="19"/>
-      <c r="G52" s="20"/>
-    </row>
-    <row r="53" ht="14.25" customHeight="1">
-      <c r="A53" s="19"/>
-      <c r="B53" s="19"/>
-      <c r="C53" s="19"/>
-      <c r="D53" s="19"/>
-      <c r="E53" s="19"/>
-      <c r="F53" s="19"/>
-      <c r="G53" s="20"/>
-    </row>
-    <row r="54" ht="14.25" customHeight="1">
-      <c r="A54" s="19"/>
-      <c r="B54" s="19"/>
-      <c r="C54" s="19"/>
-      <c r="D54" s="19"/>
-      <c r="E54" s="19"/>
-      <c r="F54" s="19"/>
-      <c r="G54" s="20"/>
-    </row>
-    <row r="55" ht="14.25" customHeight="1">
-      <c r="A55" s="19"/>
-      <c r="B55" s="19"/>
-      <c r="C55" s="19"/>
-      <c r="D55" s="19"/>
-      <c r="E55" s="19"/>
-      <c r="F55" s="19"/>
-      <c r="G55" s="20"/>
-    </row>
-    <row r="56" ht="14.25" customHeight="1">
-      <c r="A56" s="19"/>
-      <c r="B56" s="19"/>
-      <c r="C56" s="19"/>
-      <c r="D56" s="19"/>
-      <c r="E56" s="19"/>
-      <c r="F56" s="19"/>
-      <c r="G56" s="20"/>
-    </row>
-    <row r="57" ht="14.25" customHeight="1">
-      <c r="A57" s="19"/>
-      <c r="B57" s="19"/>
-      <c r="C57" s="19"/>
-      <c r="D57" s="19"/>
-      <c r="E57" s="19"/>
-      <c r="F57" s="19"/>
-      <c r="G57" s="20"/>
-    </row>
-    <row r="58" ht="14.25" customHeight="1">
-      <c r="A58" s="19"/>
-      <c r="B58" s="19"/>
-      <c r="C58" s="19"/>
-      <c r="D58" s="19"/>
-      <c r="E58" s="19"/>
-      <c r="F58" s="19"/>
-      <c r="G58" s="20"/>
-    </row>
-    <row r="59" ht="14.25" customHeight="1">
-      <c r="A59" s="19"/>
-      <c r="B59" s="19"/>
-      <c r="C59" s="19"/>
-      <c r="D59" s="19"/>
-      <c r="E59" s="19"/>
-      <c r="F59" s="19"/>
-      <c r="G59" s="20"/>
-    </row>
-    <row r="60" ht="14.25" customHeight="1">
-      <c r="A60" s="19"/>
-      <c r="B60" s="19"/>
-      <c r="C60" s="19"/>
-      <c r="D60" s="19"/>
-      <c r="E60" s="19"/>
-      <c r="F60" s="19"/>
-      <c r="G60" s="20"/>
-    </row>
-    <row r="61" ht="14.25" customHeight="1">
-      <c r="A61" s="19"/>
-      <c r="B61" s="19"/>
-      <c r="C61" s="19"/>
-      <c r="D61" s="19"/>
-      <c r="E61" s="19"/>
-      <c r="F61" s="19"/>
-      <c r="G61" s="20"/>
-    </row>
-    <row r="62" ht="14.25" customHeight="1">
-      <c r="A62" s="19"/>
-      <c r="B62" s="19"/>
-      <c r="C62" s="19"/>
-      <c r="D62" s="19"/>
-      <c r="E62" s="19"/>
-      <c r="F62" s="19"/>
-      <c r="G62" s="20"/>
-    </row>
-    <row r="63" ht="14.25" customHeight="1">
-      <c r="A63" s="19"/>
-      <c r="B63" s="19"/>
-      <c r="C63" s="19"/>
-      <c r="D63" s="19"/>
-      <c r="E63" s="19"/>
-      <c r="F63" s="19"/>
-      <c r="G63" s="20"/>
-    </row>
-    <row r="64" ht="14.25" customHeight="1">
-      <c r="A64" s="19"/>
-      <c r="B64" s="19"/>
-      <c r="C64" s="19"/>
-      <c r="D64" s="19"/>
-      <c r="E64" s="19"/>
-      <c r="F64" s="19"/>
-      <c r="G64" s="20"/>
-    </row>
-    <row r="65" ht="14.25" customHeight="1">
-      <c r="A65" s="19"/>
-      <c r="B65" s="19"/>
-      <c r="C65" s="19"/>
-      <c r="D65" s="19"/>
-      <c r="E65" s="19"/>
-      <c r="F65" s="19"/>
-      <c r="G65" s="20"/>
-    </row>
-    <row r="66" ht="14.25" customHeight="1">
-      <c r="A66" s="19"/>
-      <c r="B66" s="19"/>
-      <c r="C66" s="19"/>
-      <c r="D66" s="19"/>
-      <c r="E66" s="19"/>
-      <c r="F66" s="19"/>
-      <c r="G66" s="20"/>
-    </row>
-    <row r="67" ht="14.25" customHeight="1">
-      <c r="A67" s="19"/>
-      <c r="B67" s="19"/>
-      <c r="C67" s="19"/>
-      <c r="D67" s="19"/>
-      <c r="E67" s="19"/>
-      <c r="F67" s="19"/>
-      <c r="G67" s="20"/>
-    </row>
-    <row r="68" ht="14.25" customHeight="1">
-      <c r="A68" s="19"/>
-      <c r="B68" s="19"/>
-      <c r="C68" s="19"/>
-      <c r="D68" s="19"/>
-      <c r="E68" s="19"/>
-      <c r="F68" s="19"/>
-      <c r="G68" s="20"/>
-    </row>
-    <row r="69" ht="14.25" customHeight="1">
-      <c r="A69" s="19"/>
-      <c r="B69" s="19"/>
-      <c r="C69" s="19"/>
-      <c r="D69" s="19"/>
-      <c r="E69" s="19"/>
-      <c r="F69" s="19"/>
-      <c r="G69" s="20"/>
-    </row>
-    <row r="70" ht="14.25" customHeight="1">
-      <c r="A70" s="19"/>
-      <c r="B70" s="19"/>
-      <c r="C70" s="19"/>
-      <c r="D70" s="19"/>
-      <c r="E70" s="19"/>
-      <c r="F70" s="19"/>
-      <c r="G70" s="20"/>
-    </row>
-    <row r="71" ht="14.25" customHeight="1">
-      <c r="A71" s="19"/>
-      <c r="B71" s="19"/>
-      <c r="C71" s="19"/>
-      <c r="D71" s="19"/>
-      <c r="E71" s="19"/>
-      <c r="F71" s="19"/>
-      <c r="G71" s="20"/>
-    </row>
-    <row r="72" ht="14.25" customHeight="1">
-      <c r="A72" s="19"/>
-      <c r="B72" s="19"/>
-      <c r="C72" s="19"/>
-      <c r="D72" s="19"/>
-      <c r="E72" s="19"/>
-      <c r="F72" s="19"/>
-      <c r="G72" s="20"/>
-    </row>
-    <row r="73" ht="14.25" customHeight="1">
-      <c r="A73" s="19"/>
-      <c r="B73" s="19"/>
-      <c r="C73" s="19"/>
-      <c r="D73" s="19"/>
-      <c r="E73" s="19"/>
-      <c r="F73" s="19"/>
-      <c r="G73" s="20"/>
-    </row>
-    <row r="74" ht="14.25" customHeight="1">
-      <c r="A74" s="19"/>
-      <c r="B74" s="19"/>
-      <c r="C74" s="19"/>
-      <c r="D74" s="19"/>
-      <c r="E74" s="19"/>
-      <c r="F74" s="19"/>
-      <c r="G74" s="20"/>
-    </row>
-    <row r="75" ht="14.25" customHeight="1">
-      <c r="A75" s="19"/>
-      <c r="B75" s="19"/>
-      <c r="C75" s="19"/>
-      <c r="D75" s="19"/>
-      <c r="E75" s="19"/>
-      <c r="F75" s="19"/>
-      <c r="G75" s="20"/>
-    </row>
-    <row r="76" ht="14.25" customHeight="1">
-      <c r="A76" s="19"/>
-      <c r="B76" s="19"/>
-      <c r="C76" s="19"/>
-      <c r="D76" s="19"/>
-      <c r="E76" s="19"/>
-      <c r="F76" s="19"/>
-      <c r="G76" s="20"/>
-    </row>
-    <row r="77" ht="14.25" customHeight="1">
-      <c r="A77" s="19"/>
-      <c r="B77" s="19"/>
-      <c r="C77" s="19"/>
-      <c r="D77" s="19"/>
-      <c r="E77" s="19"/>
-      <c r="F77" s="19"/>
-      <c r="G77" s="20"/>
-    </row>
-    <row r="78" ht="14.25" customHeight="1">
-      <c r="A78" s="19"/>
-      <c r="B78" s="19"/>
-      <c r="C78" s="19"/>
-      <c r="D78" s="19"/>
-      <c r="E78" s="19"/>
-      <c r="F78" s="19"/>
-      <c r="G78" s="20"/>
-    </row>
-    <row r="79" ht="14.25" customHeight="1">
-      <c r="A79" s="19"/>
-      <c r="B79" s="19"/>
-      <c r="C79" s="19"/>
-      <c r="D79" s="19"/>
-      <c r="E79" s="19"/>
-      <c r="F79" s="19"/>
-      <c r="G79" s="20"/>
-    </row>
-    <row r="80" ht="14.25" customHeight="1">
-      <c r="A80" s="19"/>
-      <c r="B80" s="19"/>
-      <c r="C80" s="19"/>
-      <c r="D80" s="19"/>
-      <c r="E80" s="19"/>
-      <c r="F80" s="19"/>
-      <c r="G80" s="20"/>
-    </row>
-    <row r="81" ht="14.25" customHeight="1">
-      <c r="A81" s="19"/>
-      <c r="B81" s="19"/>
-      <c r="C81" s="19"/>
-      <c r="D81" s="19"/>
-      <c r="E81" s="19"/>
-      <c r="F81" s="19"/>
-      <c r="G81" s="20"/>
-    </row>
-    <row r="82" ht="14.25" customHeight="1">
-      <c r="A82" s="19"/>
-      <c r="B82" s="19"/>
-      <c r="C82" s="19"/>
-      <c r="D82" s="19"/>
-      <c r="E82" s="19"/>
-      <c r="F82" s="19"/>
-      <c r="G82" s="20"/>
-    </row>
-    <row r="83" ht="14.25" customHeight="1">
-      <c r="A83" s="19"/>
-      <c r="B83" s="19"/>
-      <c r="C83" s="19"/>
-      <c r="D83" s="19"/>
-      <c r="E83" s="19"/>
-      <c r="F83" s="19"/>
-      <c r="G83" s="20"/>
-    </row>
-    <row r="84" ht="14.25" customHeight="1">
-      <c r="A84" s="19"/>
-      <c r="B84" s="19"/>
-      <c r="C84" s="19"/>
-      <c r="D84" s="19"/>
-      <c r="E84" s="19"/>
-      <c r="F84" s="19"/>
-      <c r="G84" s="20"/>
-    </row>
-    <row r="85" ht="14.25" customHeight="1">
-      <c r="A85" s="19"/>
-      <c r="B85" s="19"/>
-      <c r="C85" s="19"/>
-      <c r="D85" s="19"/>
-      <c r="E85" s="19"/>
-      <c r="F85" s="19"/>
-      <c r="G85" s="20"/>
-    </row>
-    <row r="86" ht="14.25" customHeight="1">
-      <c r="A86" s="19"/>
-      <c r="B86" s="19"/>
-      <c r="C86" s="19"/>
-      <c r="D86" s="19"/>
-      <c r="E86" s="19"/>
-      <c r="F86" s="19"/>
-      <c r="G86" s="20"/>
-    </row>
-    <row r="87" ht="14.25" customHeight="1">
-      <c r="A87" s="19"/>
-      <c r="B87" s="19"/>
-      <c r="C87" s="19"/>
-      <c r="D87" s="19"/>
-      <c r="E87" s="19"/>
-      <c r="F87" s="19"/>
-      <c r="G87" s="20"/>
-    </row>
-    <row r="88" ht="14.25" customHeight="1">
-      <c r="A88" s="19"/>
-      <c r="B88" s="19"/>
-      <c r="C88" s="19"/>
-      <c r="D88" s="19"/>
-      <c r="E88" s="19"/>
-      <c r="F88" s="19"/>
-      <c r="G88" s="20"/>
-    </row>
-    <row r="89" ht="14.25" customHeight="1">
-      <c r="A89" s="19"/>
-      <c r="B89" s="19"/>
-      <c r="C89" s="19"/>
-      <c r="D89" s="19"/>
-      <c r="E89" s="19"/>
-      <c r="F89" s="19"/>
-      <c r="G89" s="20"/>
-    </row>
-    <row r="90" ht="14.25" customHeight="1">
-      <c r="A90" s="19"/>
-      <c r="B90" s="19"/>
-      <c r="C90" s="19"/>
-      <c r="D90" s="19"/>
-      <c r="E90" s="19"/>
-      <c r="F90" s="19"/>
-      <c r="G90" s="20"/>
-    </row>
-    <row r="91" ht="14.25" customHeight="1">
-      <c r="A91" s="19"/>
-      <c r="B91" s="19"/>
-      <c r="C91" s="19"/>
-      <c r="D91" s="19"/>
-      <c r="E91" s="19"/>
-      <c r="F91" s="19"/>
-      <c r="G91" s="20"/>
-    </row>
-    <row r="92" ht="14.25" customHeight="1">
-      <c r="A92" s="19"/>
-      <c r="B92" s="19"/>
-      <c r="C92" s="19"/>
-      <c r="D92" s="19"/>
-      <c r="E92" s="19"/>
-      <c r="F92" s="19"/>
-      <c r="G92" s="20"/>
-    </row>
-    <row r="93" ht="14.25" customHeight="1">
-      <c r="A93" s="19"/>
-      <c r="B93" s="19"/>
-      <c r="C93" s="19"/>
-      <c r="D93" s="19"/>
-      <c r="E93" s="19"/>
-      <c r="F93" s="19"/>
-      <c r="G93" s="20"/>
-    </row>
-    <row r="94" ht="14.25" customHeight="1">
-      <c r="A94" s="19"/>
-      <c r="B94" s="19"/>
-      <c r="C94" s="19"/>
-      <c r="D94" s="19"/>
-      <c r="E94" s="19"/>
-      <c r="F94" s="19"/>
-      <c r="G94" s="20"/>
-    </row>
-    <row r="95" ht="14.25" customHeight="1">
-      <c r="A95" s="19"/>
-      <c r="B95" s="19"/>
-      <c r="C95" s="19"/>
-      <c r="D95" s="19"/>
-      <c r="E95" s="19"/>
-      <c r="F95" s="19"/>
-      <c r="G95" s="20"/>
-    </row>
-    <row r="96" ht="14.25" customHeight="1">
-      <c r="A96" s="19"/>
-      <c r="B96" s="19"/>
-      <c r="C96" s="19"/>
-      <c r="D96" s="19"/>
-      <c r="E96" s="19"/>
-      <c r="F96" s="19"/>
-      <c r="G96" s="20"/>
-    </row>
-    <row r="97" ht="14.25" customHeight="1">
-      <c r="A97" s="19"/>
-      <c r="B97" s="19"/>
-      <c r="C97" s="19"/>
-      <c r="D97" s="19"/>
-      <c r="E97" s="19"/>
-      <c r="F97" s="19"/>
-      <c r="G97" s="20"/>
-    </row>
-    <row r="98" ht="14.25" customHeight="1">
-      <c r="A98" s="19"/>
-      <c r="B98" s="19"/>
-      <c r="C98" s="19"/>
-      <c r="D98" s="19"/>
-      <c r="E98" s="19"/>
-      <c r="F98" s="19"/>
-      <c r="G98" s="20"/>
-    </row>
-    <row r="99" ht="14.25" customHeight="1">
-      <c r="A99" s="19"/>
-      <c r="B99" s="19"/>
-      <c r="C99" s="19"/>
-      <c r="D99" s="19"/>
-      <c r="E99" s="19"/>
-      <c r="F99" s="19"/>
-      <c r="G99" s="20"/>
-    </row>
-    <row r="100" ht="14.25" customHeight="1">
-      <c r="A100" s="19"/>
-      <c r="B100" s="19"/>
-      <c r="C100" s="19"/>
-      <c r="D100" s="19"/>
-      <c r="E100" s="19"/>
-      <c r="F100" s="19"/>
-      <c r="G100" s="20"/>
-    </row>
-    <row r="101" ht="14.25" customHeight="1">
-      <c r="A101" s="19"/>
-      <c r="B101" s="19"/>
-      <c r="C101" s="19"/>
-      <c r="D101" s="19"/>
-      <c r="E101" s="19"/>
-      <c r="F101" s="19"/>
-      <c r="G101" s="20"/>
-    </row>
-    <row r="102" ht="14.25" customHeight="1">
-      <c r="A102" s="19"/>
-      <c r="B102" s="19"/>
-      <c r="C102" s="19"/>
-      <c r="D102" s="19"/>
-      <c r="E102" s="19"/>
-      <c r="F102" s="19"/>
-      <c r="G102" s="20"/>
-    </row>
-    <row r="103" ht="14.25" customHeight="1">
-      <c r="A103" s="19"/>
-      <c r="B103" s="19"/>
-      <c r="C103" s="19"/>
-      <c r="D103" s="19"/>
-      <c r="E103" s="19"/>
-      <c r="F103" s="19"/>
-      <c r="G103" s="20"/>
-    </row>
-    <row r="104" ht="14.25" customHeight="1">
-      <c r="A104" s="19"/>
-      <c r="B104" s="19"/>
-      <c r="C104" s="19"/>
-      <c r="D104" s="19"/>
-      <c r="E104" s="19"/>
-      <c r="F104" s="19"/>
-      <c r="G104" s="20"/>
-    </row>
-    <row r="105" ht="14.25" customHeight="1">
-      <c r="A105" s="19"/>
-      <c r="B105" s="19"/>
-      <c r="C105" s="19"/>
-      <c r="D105" s="19"/>
-      <c r="E105" s="19"/>
-      <c r="F105" s="19"/>
-      <c r="G105" s="20"/>
-    </row>
-    <row r="106" ht="14.25" customHeight="1">
-      <c r="A106" s="19"/>
-      <c r="B106" s="19"/>
-      <c r="C106" s="19"/>
-      <c r="D106" s="19"/>
-      <c r="E106" s="19"/>
-      <c r="F106" s="19"/>
-      <c r="G106" s="20"/>
-    </row>
-    <row r="107" ht="14.25" customHeight="1">
-      <c r="A107" s="19"/>
-      <c r="B107" s="19"/>
-      <c r="C107" s="19"/>
-      <c r="D107" s="19"/>
-      <c r="E107" s="19"/>
-      <c r="F107" s="19"/>
-      <c r="G107" s="20"/>
-    </row>
-    <row r="108" ht="14.25" customHeight="1">
-      <c r="A108" s="19"/>
-      <c r="B108" s="19"/>
-      <c r="C108" s="19"/>
-      <c r="D108" s="19"/>
-      <c r="E108" s="19"/>
-      <c r="F108" s="19"/>
-      <c r="G108" s="20"/>
-    </row>
-    <row r="109" ht="14.25" customHeight="1">
-      <c r="A109" s="19"/>
-      <c r="B109" s="19"/>
-      <c r="C109" s="19"/>
-      <c r="D109" s="19"/>
-      <c r="E109" s="19"/>
-      <c r="F109" s="19"/>
-      <c r="G109" s="20"/>
-    </row>
-    <row r="110" ht="14.25" customHeight="1">
-      <c r="A110" s="19"/>
-      <c r="B110" s="19"/>
-      <c r="C110" s="19"/>
-      <c r="D110" s="19"/>
-      <c r="E110" s="19"/>
-      <c r="F110" s="19"/>
-      <c r="G110" s="20"/>
-    </row>
-    <row r="111" ht="14.25" customHeight="1">
-      <c r="A111" s="19"/>
-      <c r="B111" s="19"/>
-      <c r="C111" s="19"/>
-      <c r="D111" s="19"/>
-      <c r="E111" s="19"/>
-      <c r="F111" s="19"/>
-      <c r="G111" s="20"/>
-    </row>
-    <row r="112" ht="14.25" customHeight="1">
-      <c r="A112" s="19"/>
-      <c r="B112" s="19"/>
-      <c r="C112" s="19"/>
-      <c r="D112" s="19"/>
-      <c r="E112" s="19"/>
-      <c r="F112" s="19"/>
-      <c r="G112" s="20"/>
-    </row>
-    <row r="113" ht="14.25" customHeight="1">
-      <c r="A113" s="19"/>
-      <c r="B113" s="19"/>
-      <c r="C113" s="19"/>
-      <c r="D113" s="19"/>
-      <c r="E113" s="19"/>
-      <c r="F113" s="19"/>
-      <c r="G113" s="20"/>
-    </row>
-    <row r="114" ht="14.25" customHeight="1">
-      <c r="A114" s="19"/>
-      <c r="B114" s="19"/>
-      <c r="C114" s="19"/>
-      <c r="D114" s="19"/>
-      <c r="E114" s="19"/>
-      <c r="F114" s="19"/>
-      <c r="G114" s="20"/>
-    </row>
-    <row r="115" ht="14.25" customHeight="1">
-      <c r="A115" s="19"/>
-      <c r="B115" s="19"/>
-      <c r="C115" s="19"/>
-      <c r="D115" s="19"/>
-      <c r="E115" s="19"/>
-      <c r="F115" s="19"/>
-      <c r="G115" s="20"/>
-    </row>
-    <row r="116" ht="14.25" customHeight="1">
-      <c r="A116" s="19"/>
-      <c r="B116" s="19"/>
-      <c r="C116" s="19"/>
-      <c r="D116" s="19"/>
-      <c r="E116" s="19"/>
-      <c r="F116" s="19"/>
-      <c r="G116" s="20"/>
-    </row>
-    <row r="117" ht="14.25" customHeight="1">
-      <c r="A117" s="19"/>
-      <c r="B117" s="19"/>
-      <c r="C117" s="19"/>
-      <c r="D117" s="19"/>
-      <c r="E117" s="19"/>
-      <c r="F117" s="19"/>
-      <c r="G117" s="20"/>
-    </row>
-    <row r="118" ht="14.25" customHeight="1">
-      <c r="A118" s="19"/>
-      <c r="B118" s="19"/>
-      <c r="C118" s="19"/>
-      <c r="D118" s="19"/>
-      <c r="E118" s="19"/>
-      <c r="F118" s="19"/>
-      <c r="G118" s="20"/>
-    </row>
-    <row r="119" ht="14.25" customHeight="1">
-      <c r="A119" s="19"/>
-      <c r="B119" s="19"/>
-      <c r="C119" s="19"/>
-      <c r="D119" s="19"/>
-      <c r="E119" s="19"/>
-      <c r="F119" s="19"/>
-      <c r="G119" s="20"/>
-    </row>
-    <row r="120" ht="14.25" customHeight="1">
-      <c r="A120" s="19"/>
-      <c r="B120" s="19"/>
-      <c r="C120" s="19"/>
-      <c r="D120" s="19"/>
-      <c r="E120" s="19"/>
-      <c r="F120" s="19"/>
-      <c r="G120" s="20"/>
-    </row>
-    <row r="121" ht="14.25" customHeight="1">
-      <c r="A121" s="19"/>
-      <c r="B121" s="19"/>
-      <c r="C121" s="19"/>
-      <c r="D121" s="19"/>
-      <c r="E121" s="19"/>
-      <c r="F121" s="19"/>
-      <c r="G121" s="20"/>
-    </row>
-    <row r="122" ht="14.25" customHeight="1">
-      <c r="A122" s="19"/>
-      <c r="B122" s="19"/>
-      <c r="C122" s="19"/>
-      <c r="D122" s="19"/>
-      <c r="E122" s="19"/>
-      <c r="F122" s="19"/>
-      <c r="G122" s="20"/>
-    </row>
-    <row r="123" ht="14.25" customHeight="1">
-      <c r="A123" s="19"/>
-      <c r="B123" s="19"/>
-      <c r="C123" s="19"/>
-      <c r="D123" s="19"/>
-      <c r="E123" s="19"/>
-      <c r="F123" s="19"/>
-      <c r="G123" s="20"/>
-    </row>
-    <row r="124" ht="14.25" customHeight="1">
-      <c r="A124" s="19"/>
-      <c r="B124" s="19"/>
-      <c r="C124" s="19"/>
-      <c r="D124" s="19"/>
-      <c r="E124" s="19"/>
-      <c r="F124" s="19"/>
-      <c r="G124" s="20"/>
-    </row>
-    <row r="125" ht="14.25" customHeight="1">
-      <c r="A125" s="19"/>
-      <c r="B125" s="19"/>
-      <c r="C125" s="19"/>
-      <c r="D125" s="19"/>
-      <c r="E125" s="19"/>
-      <c r="F125" s="19"/>
-      <c r="G125" s="20"/>
-    </row>
+      <c r="A22" s="22"/>
+      <c r="B22" s="22"/>
+      <c r="C22" s="22"/>
+      <c r="D22" s="22"/>
+      <c r="E22" s="22"/>
+      <c r="F22" s="22"/>
+      <c r="G22" s="23"/>
+    </row>
+    <row r="23" ht="14.25" customHeight="1"/>
+    <row r="24" ht="14.25" customHeight="1"/>
+    <row r="25" ht="14.25" customHeight="1"/>
+    <row r="26" ht="14.25" customHeight="1"/>
+    <row r="27" ht="14.25" customHeight="1"/>
+    <row r="28" ht="14.25" customHeight="1"/>
+    <row r="29" ht="14.25" customHeight="1"/>
+    <row r="30" ht="14.25" customHeight="1"/>
+    <row r="31" ht="14.25" customHeight="1"/>
+    <row r="32" ht="14.25" customHeight="1"/>
+    <row r="33" ht="14.25" customHeight="1"/>
+    <row r="34" ht="14.25" customHeight="1"/>
+    <row r="35" ht="14.25" customHeight="1"/>
+    <row r="36" ht="14.25" customHeight="1"/>
+    <row r="37" ht="14.25" customHeight="1"/>
+    <row r="38" ht="14.25" customHeight="1"/>
+    <row r="39" ht="14.25" customHeight="1"/>
+    <row r="40" ht="14.25" customHeight="1"/>
+    <row r="41" ht="14.25" customHeight="1"/>
+    <row r="42" ht="14.25" customHeight="1"/>
+    <row r="43" ht="14.25" customHeight="1"/>
+    <row r="44" ht="14.25" customHeight="1"/>
+    <row r="45" ht="14.25" customHeight="1"/>
+    <row r="46" ht="14.25" customHeight="1"/>
+    <row r="47" ht="14.25" customHeight="1"/>
+    <row r="48" ht="14.25" customHeight="1"/>
+    <row r="49" ht="14.25" customHeight="1"/>
+    <row r="50" ht="14.25" customHeight="1"/>
+    <row r="51" ht="14.25" customHeight="1"/>
+    <row r="52" ht="14.25" customHeight="1"/>
+    <row r="53" ht="14.25" customHeight="1"/>
+    <row r="54" ht="14.25" customHeight="1"/>
+    <row r="55" ht="14.25" customHeight="1"/>
+    <row r="56" ht="14.25" customHeight="1"/>
+    <row r="57" ht="14.25" customHeight="1"/>
+    <row r="58" ht="14.25" customHeight="1"/>
+    <row r="59" ht="14.25" customHeight="1"/>
+    <row r="60" ht="14.25" customHeight="1"/>
+    <row r="61" ht="14.25" customHeight="1"/>
+    <row r="62" ht="14.25" customHeight="1"/>
+    <row r="63" ht="14.25" customHeight="1"/>
+    <row r="64" ht="14.25" customHeight="1"/>
+    <row r="65" ht="14.25" customHeight="1"/>
+    <row r="66" ht="14.25" customHeight="1"/>
+    <row r="67" ht="14.25" customHeight="1"/>
+    <row r="68" ht="14.25" customHeight="1"/>
+    <row r="69" ht="14.25" customHeight="1"/>
+    <row r="70" ht="14.25" customHeight="1"/>
+    <row r="71" ht="14.25" customHeight="1"/>
+    <row r="72" ht="14.25" customHeight="1"/>
+    <row r="73" ht="14.25" customHeight="1"/>
+    <row r="74" ht="14.25" customHeight="1"/>
+    <row r="75" ht="14.25" customHeight="1"/>
+    <row r="76" ht="14.25" customHeight="1"/>
+    <row r="77" ht="14.25" customHeight="1"/>
+    <row r="78" ht="14.25" customHeight="1"/>
+    <row r="79" ht="14.25" customHeight="1"/>
+    <row r="80" ht="14.25" customHeight="1"/>
+    <row r="81" ht="14.25" customHeight="1"/>
+    <row r="82" ht="14.25" customHeight="1"/>
+    <row r="83" ht="14.25" customHeight="1"/>
+    <row r="84" ht="14.25" customHeight="1"/>
+    <row r="85" ht="14.25" customHeight="1"/>
+    <row r="86" ht="14.25" customHeight="1"/>
+    <row r="87" ht="14.25" customHeight="1"/>
+    <row r="88" ht="14.25" customHeight="1"/>
+    <row r="89" ht="14.25" customHeight="1"/>
+    <row r="90" ht="14.25" customHeight="1"/>
+    <row r="91" ht="14.25" customHeight="1"/>
+    <row r="92" ht="14.25" customHeight="1"/>
+    <row r="93" ht="14.25" customHeight="1"/>
+    <row r="94" ht="14.25" customHeight="1"/>
+    <row r="95" ht="14.25" customHeight="1"/>
+    <row r="96" ht="14.25" customHeight="1"/>
+    <row r="97" ht="14.25" customHeight="1"/>
+    <row r="98" ht="14.25" customHeight="1"/>
+    <row r="99" ht="14.25" customHeight="1"/>
+    <row r="100" ht="14.25" customHeight="1"/>
+    <row r="101" ht="14.25" customHeight="1"/>
+    <row r="102" ht="14.25" customHeight="1"/>
+    <row r="103" ht="14.25" customHeight="1"/>
+    <row r="104" ht="14.25" customHeight="1"/>
+    <row r="105" ht="14.25" customHeight="1"/>
+    <row r="106" ht="14.25" customHeight="1"/>
+    <row r="107" ht="14.25" customHeight="1"/>
+    <row r="108" ht="14.25" customHeight="1"/>
+    <row r="109" ht="14.25" customHeight="1"/>
+    <row r="110" ht="14.25" customHeight="1"/>
+    <row r="111" ht="14.25" customHeight="1"/>
+    <row r="112" ht="14.25" customHeight="1"/>
+    <row r="113" ht="14.25" customHeight="1"/>
+    <row r="114" ht="14.25" customHeight="1"/>
+    <row r="115" ht="14.25" customHeight="1"/>
+    <row r="116" ht="14.25" customHeight="1"/>
+    <row r="117" ht="14.25" customHeight="1"/>
+    <row r="118" ht="14.25" customHeight="1"/>
+    <row r="119" ht="14.25" customHeight="1"/>
+    <row r="120" ht="14.25" customHeight="1"/>
+    <row r="121" ht="14.25" customHeight="1"/>
+    <row r="122" ht="14.25" customHeight="1"/>
+    <row r="123" ht="14.25" customHeight="1"/>
+    <row r="124" ht="14.25" customHeight="1"/>
+    <row r="125" ht="14.25" customHeight="1"/>
     <row r="126" ht="14.25" customHeight="1"/>
     <row r="127" ht="14.25" customHeight="1"/>
     <row r="128" ht="14.25" customHeight="1"/>
@@ -2735,8 +2054,8 @@
     <hyperlink r:id="rId1" ref="B6"/>
   </hyperlinks>
   <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait"/>
+  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.25" right="0.25" top="0.75"/>
+  <pageSetup orientation="landscape"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added all diary entries for the past 2 weeks
</commit_message>
<xml_diff>
--- a/diaries/diary-chunqi-zhao.xlsx
+++ b/diaries/diary-chunqi-zhao.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="84">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -212,6 +212,63 @@
   </si>
   <si>
     <t>Good, ready for class.</t>
+  </si>
+  <si>
+    <t>9:00PM - 1:00AM</t>
+  </si>
+  <si>
+    <t>Study for the midterm</t>
+  </si>
+  <si>
+    <t>Hopefully memorized everything</t>
+  </si>
+  <si>
+    <t>There weren't a ton of materials so I should be fine</t>
+  </si>
+  <si>
+    <t>Decent, tired</t>
+  </si>
+  <si>
+    <t>5:00 PM - 7:50PM</t>
+  </si>
+  <si>
+    <t>Take midterm, and learn</t>
+  </si>
+  <si>
+    <t>Did okay on the midterm I think, Learned about the stakeholders, functionalities, and key developers of a project</t>
+  </si>
+  <si>
+    <t>Finding all these should be easy for Runelite, since I am very familiar with the game and the client</t>
+  </si>
+  <si>
+    <t>Exhausted from the midterm</t>
+  </si>
+  <si>
+    <t>9:00PM - 2:00AM</t>
+  </si>
+  <si>
+    <t>Work on the Big Picture</t>
+  </si>
+  <si>
+    <t>Was able to identify everything and explain them all</t>
+  </si>
+  <si>
+    <t>Instructions were clear, but not sure if bullet point answers would suffice, so we tried to explain everything in detail</t>
+  </si>
+  <si>
+    <t>Confused?</t>
+  </si>
+  <si>
+    <t>3:00PM - 5:00PM</t>
+  </si>
+  <si>
+    <t>Finishing touches to the homework</t>
+  </si>
+  <si>
+    <t>Nothing much to reflect on, hopefully meets expectations</t>
+  </si>
+  <si>
+    <t>Uncertain?</t>
   </si>
 </sst>
 </file>
@@ -222,7 +279,7 @@
     <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
     <numFmt numFmtId="165" formatCode="h:mm am/pm"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="13">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -277,6 +334,12 @@
       <i/>
       <sz val="11.0"/>
       <color rgb="FF006100"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12.0"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="5">
@@ -446,10 +509,10 @@
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="10" fillId="4" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
+      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="10" fillId="4" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
+    <xf borderId="10" fillId="4" fontId="12" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1060,23 +1123,151 @@
       </c>
     </row>
     <row r="22" ht="14.25" customHeight="1">
-      <c r="A22" s="22"/>
-      <c r="B22" s="22"/>
-      <c r="C22" s="22"/>
-      <c r="D22" s="22"/>
-      <c r="E22" s="22"/>
-      <c r="F22" s="22"/>
-      <c r="G22" s="23"/>
-    </row>
-    <row r="23" ht="14.25" customHeight="1"/>
-    <row r="24" ht="14.25" customHeight="1"/>
-    <row r="25" ht="14.25" customHeight="1"/>
-    <row r="26" ht="14.25" customHeight="1"/>
-    <row r="27" ht="14.25" customHeight="1"/>
-    <row r="28" ht="14.25" customHeight="1"/>
-    <row r="29" ht="14.25" customHeight="1"/>
-    <row r="30" ht="14.25" customHeight="1"/>
-    <row r="31" ht="14.25" customHeight="1"/>
+      <c r="A22" s="18">
+        <v>43873.0</v>
+      </c>
+      <c r="B22" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="C22" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D22" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="E22" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="F22" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="G22" s="21" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="23" ht="14.25" customHeight="1">
+      <c r="A23" s="18">
+        <v>43874.0</v>
+      </c>
+      <c r="B23" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="C23" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D23" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="E23" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="F23" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="G23" s="20" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="24" ht="14.25" customHeight="1">
+      <c r="A24" s="18">
+        <v>43880.0</v>
+      </c>
+      <c r="B24" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="C24" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="D24" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="E24" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="F24" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="G24" s="20" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="25" ht="14.25" customHeight="1">
+      <c r="A25" s="18">
+        <v>43881.0</v>
+      </c>
+      <c r="B25" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="C25" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="D25" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="E25" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="F25" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="G25" s="20" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="26" ht="14.25" customHeight="1">
+      <c r="A26" s="23"/>
+      <c r="B26" s="22"/>
+      <c r="C26" s="23"/>
+      <c r="D26" s="23"/>
+      <c r="E26" s="23"/>
+      <c r="F26" s="23"/>
+      <c r="G26" s="23"/>
+    </row>
+    <row r="27" ht="14.25" customHeight="1">
+      <c r="A27" s="23"/>
+      <c r="B27" s="22"/>
+      <c r="C27" s="23"/>
+      <c r="D27" s="23"/>
+      <c r="E27" s="23"/>
+      <c r="F27" s="23"/>
+      <c r="G27" s="23"/>
+    </row>
+    <row r="28" ht="14.25" customHeight="1">
+      <c r="A28" s="23"/>
+      <c r="B28" s="22"/>
+      <c r="C28" s="23"/>
+      <c r="D28" s="23"/>
+      <c r="E28" s="23"/>
+      <c r="F28" s="23"/>
+      <c r="G28" s="23"/>
+    </row>
+    <row r="29" ht="14.25" customHeight="1">
+      <c r="A29" s="23"/>
+      <c r="B29" s="22"/>
+      <c r="C29" s="23"/>
+      <c r="D29" s="23"/>
+      <c r="E29" s="23"/>
+      <c r="F29" s="23"/>
+      <c r="G29" s="23"/>
+    </row>
+    <row r="30" ht="14.25" customHeight="1">
+      <c r="A30" s="23"/>
+      <c r="B30" s="22"/>
+      <c r="C30" s="20"/>
+      <c r="D30" s="23"/>
+      <c r="E30" s="23"/>
+      <c r="F30" s="23"/>
+      <c r="G30" s="23"/>
+    </row>
+    <row r="31" ht="14.25" customHeight="1">
+      <c r="A31" s="23"/>
+      <c r="B31" s="22"/>
+      <c r="C31" s="23"/>
+      <c r="D31" s="23"/>
+      <c r="E31" s="23"/>
+      <c r="F31" s="23"/>
+      <c r="G31" s="23"/>
+    </row>
     <row r="32" ht="14.25" customHeight="1"/>
     <row r="33" ht="14.25" customHeight="1"/>
     <row r="34" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
add diary for week 7
</commit_message>
<xml_diff>
--- a/diaries/diary-chunqi-zhao.xlsx
+++ b/diaries/diary-chunqi-zhao.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="102">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -269,6 +269,60 @@
   </si>
   <si>
     <t>Uncertain?</t>
+  </si>
+  <si>
+    <t>5:00PM - 8:00PM</t>
+  </si>
+  <si>
+    <t>Learn something from class</t>
+  </si>
+  <si>
+    <t>Learned about how to abstract out the architecture from a system</t>
+  </si>
+  <si>
+    <t>Runelite should be fairly easy to do for us as its structure is very well defined.</t>
+  </si>
+  <si>
+    <t>Decent</t>
+  </si>
+  <si>
+    <t>4:00PM - 6:00PM</t>
+  </si>
+  <si>
+    <t>Find and document architeture for runelite</t>
+  </si>
+  <si>
+    <t>Was able to contact the devs directly and get advice on generating architecture diagram</t>
+  </si>
+  <si>
+    <t>Was surprised the devs are this responsive on their official discord server, especially the creator of the project being able to directly answer my questions felt great.</t>
+  </si>
+  <si>
+    <t>Great</t>
+  </si>
+  <si>
+    <t>Find and document social context and contribution guidelines for runelite</t>
+  </si>
+  <si>
+    <t>Was able to scrape a lot of info from their github page, and official website.</t>
+  </si>
+  <si>
+    <t>Having a well maintained project that is still ongoing helps alot with getting such info, especially when I have been using it for over 3 years</t>
+  </si>
+  <si>
+    <t>9:00PM - 5:00AM</t>
+  </si>
+  <si>
+    <t>Find interesting pull requests and issues, and document them. Reformat the document.</t>
+  </si>
+  <si>
+    <t>Found a lot of interesting stuff happening in the official github.</t>
+  </si>
+  <si>
+    <t>Some issues can only be solved by the community, some pull requests were denied and closed, learned a lot of what the maintainers are expecting from each contribution</t>
+  </si>
+  <si>
+    <t>exhausted</t>
   </si>
 </sst>
 </file>
@@ -1215,40 +1269,96 @@
       </c>
     </row>
     <row r="26" ht="14.25" customHeight="1">
-      <c r="A26" s="23"/>
-      <c r="B26" s="22"/>
-      <c r="C26" s="23"/>
-      <c r="D26" s="23"/>
-      <c r="E26" s="23"/>
-      <c r="F26" s="23"/>
-      <c r="G26" s="23"/>
+      <c r="A26" s="18">
+        <v>43881.0</v>
+      </c>
+      <c r="B26" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="C26" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D26" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="E26" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="F26" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="G26" s="20" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="27" ht="14.25" customHeight="1">
-      <c r="A27" s="23"/>
-      <c r="B27" s="22"/>
-      <c r="C27" s="23"/>
-      <c r="D27" s="23"/>
-      <c r="E27" s="23"/>
-      <c r="F27" s="23"/>
-      <c r="G27" s="23"/>
+      <c r="A27" s="18">
+        <v>43885.0</v>
+      </c>
+      <c r="B27" s="22" t="s">
+        <v>89</v>
+      </c>
+      <c r="C27" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="D27" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="E27" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="F27" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="G27" s="20" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="28" ht="14.25" customHeight="1">
-      <c r="A28" s="23"/>
-      <c r="B28" s="22"/>
-      <c r="C28" s="23"/>
-      <c r="D28" s="23"/>
-      <c r="E28" s="23"/>
-      <c r="F28" s="23"/>
-      <c r="G28" s="23"/>
+      <c r="A28" s="18">
+        <v>43886.0</v>
+      </c>
+      <c r="B28" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="C28" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="D28" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="E28" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="F28" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="G28" s="20" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="29" ht="14.25" customHeight="1">
-      <c r="A29" s="23"/>
-      <c r="B29" s="22"/>
-      <c r="C29" s="23"/>
-      <c r="D29" s="23"/>
-      <c r="E29" s="23"/>
-      <c r="F29" s="23"/>
-      <c r="G29" s="23"/>
+      <c r="A29" s="18">
+        <v>43887.0</v>
+      </c>
+      <c r="B29" s="22" t="s">
+        <v>97</v>
+      </c>
+      <c r="C29" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="D29" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="E29" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="F29" s="20" t="s">
+        <v>100</v>
+      </c>
+      <c r="G29" s="20" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="30" ht="14.25" customHeight="1">
       <c r="A30" s="23"/>

</xml_diff>

<commit_message>
add diary for week 8
</commit_message>
<xml_diff>
--- a/diaries/diary-chunqi-zhao.xlsx
+++ b/diaries/diary-chunqi-zhao.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="115">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -323,6 +323,45 @@
   </si>
   <si>
     <t>exhausted</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Learned about all kinds of different design patterns </t>
+  </si>
+  <si>
+    <t>Hopefully we are able to find these design patterns easily within Runelite, high hopes due to Runelite's good structure</t>
+  </si>
+  <si>
+    <t>hopeful</t>
+  </si>
+  <si>
+    <t>11:00AM - 1:00PM</t>
+  </si>
+  <si>
+    <t>Submit a pull request to Runelite</t>
+  </si>
+  <si>
+    <t>After actively playing the game for hours beforehand, I was finally able to get a location that wasn't centered and able to contribute with the pull request.</t>
+  </si>
+  <si>
+    <t>Commiting and submitting the pull request was the easy part, actually getting to that point was the hard part, which is the nature of this issue</t>
+  </si>
+  <si>
+    <t>Feels good that I can actually contribute to Runelite</t>
+  </si>
+  <si>
+    <t>10:00PM - 4:00AM</t>
+  </si>
+  <si>
+    <t>Find 5 design patterns in Runelite and write up on the pull request</t>
+  </si>
+  <si>
+    <t>Patterns were split up and were all found, pull request submitted earlier was merged by Runelite's team</t>
+  </si>
+  <si>
+    <t>Runelite's amazing structure saves us once again in helping us finding design patterns, since they were really clear and easy to find, the java design patterns github link posted on slack was very helpful</t>
+  </si>
+  <si>
+    <t>Tired</t>
   </si>
 </sst>
 </file>
@@ -350,15 +389,18 @@
       <b/>
       <sz val="12.0"/>
       <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
     </font>
     <font>
       <sz val="11.0"/>
       <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
     </font>
     <font>
       <i/>
       <sz val="12.0"/>
       <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
     </font>
     <font>
       <i/>
@@ -369,31 +411,35 @@
     <font>
       <sz val="12.0"/>
       <color rgb="FF006100"/>
+      <name val="Calibri"/>
     </font>
     <font>
       <sz val="11.0"/>
       <color rgb="FF006100"/>
+      <name val="Calibri"/>
     </font>
     <font>
       <b/>
       <sz val="12.0"/>
       <color rgb="FF006100"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="12.0"/>
-      <color rgb="FF006100"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11.0"/>
-      <color rgb="FF006100"/>
+      <name val="Calibri"/>
     </font>
     <font>
       <i/>
       <sz val="12.0"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11.0"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12.0"/>
+      <color rgb="FF006100"/>
     </font>
   </fonts>
   <fills count="5">
@@ -505,7 +551,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -566,6 +612,12 @@
       <alignment horizontal="right" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="10" fillId="4" fontId="12" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="10" fillId="4" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="10" fillId="4" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1269,120 +1321,202 @@
       </c>
     </row>
     <row r="26" ht="14.25" customHeight="1">
-      <c r="A26" s="18">
+      <c r="A26" s="23">
         <v>43881.0</v>
       </c>
-      <c r="B26" s="22" t="s">
+      <c r="B26" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="C26" s="20" t="s">
+      <c r="C26" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="D26" s="20" t="s">
+      <c r="D26" s="25" t="s">
         <v>85</v>
       </c>
-      <c r="E26" s="20" t="s">
+      <c r="E26" s="25" t="s">
         <v>86</v>
       </c>
-      <c r="F26" s="20" t="s">
+      <c r="F26" s="25" t="s">
         <v>87</v>
       </c>
-      <c r="G26" s="20" t="s">
+      <c r="G26" s="25" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="27" ht="14.25" customHeight="1">
-      <c r="A27" s="18">
+      <c r="A27" s="23">
         <v>43885.0</v>
       </c>
-      <c r="B27" s="22" t="s">
+      <c r="B27" s="24" t="s">
         <v>89</v>
       </c>
-      <c r="C27" s="20" t="s">
+      <c r="C27" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="D27" s="20" t="s">
+      <c r="D27" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="E27" s="20" t="s">
+      <c r="E27" s="25" t="s">
         <v>91</v>
       </c>
-      <c r="F27" s="20" t="s">
+      <c r="F27" s="25" t="s">
         <v>92</v>
       </c>
-      <c r="G27" s="20" t="s">
+      <c r="G27" s="25" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="28" ht="14.25" customHeight="1">
-      <c r="A28" s="18">
+      <c r="A28" s="23">
         <v>43886.0</v>
       </c>
-      <c r="B28" s="22" t="s">
+      <c r="B28" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="C28" s="20" t="s">
+      <c r="C28" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="D28" s="20" t="s">
+      <c r="D28" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="E28" s="20" t="s">
+      <c r="E28" s="25" t="s">
         <v>95</v>
       </c>
-      <c r="F28" s="20" t="s">
+      <c r="F28" s="25" t="s">
         <v>96</v>
       </c>
-      <c r="G28" s="20" t="s">
+      <c r="G28" s="25" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="29" ht="14.25" customHeight="1">
-      <c r="A29" s="18">
+      <c r="A29" s="23">
         <v>43887.0</v>
       </c>
-      <c r="B29" s="22" t="s">
+      <c r="B29" s="24" t="s">
         <v>97</v>
       </c>
-      <c r="C29" s="20" t="s">
+      <c r="C29" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="D29" s="20" t="s">
+      <c r="D29" s="25" t="s">
         <v>98</v>
       </c>
-      <c r="E29" s="20" t="s">
+      <c r="E29" s="25" t="s">
         <v>99</v>
       </c>
-      <c r="F29" s="20" t="s">
+      <c r="F29" s="25" t="s">
         <v>100</v>
       </c>
-      <c r="G29" s="20" t="s">
+      <c r="G29" s="25" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="30" ht="14.25" customHeight="1">
-      <c r="A30" s="23"/>
-      <c r="B30" s="22"/>
-      <c r="C30" s="20"/>
-      <c r="D30" s="23"/>
-      <c r="E30" s="23"/>
-      <c r="F30" s="23"/>
-      <c r="G30" s="23"/>
+      <c r="A30" s="23">
+        <v>43888.0</v>
+      </c>
+      <c r="B30" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="C30" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="D30" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="E30" s="25" t="s">
+        <v>102</v>
+      </c>
+      <c r="F30" s="25" t="s">
+        <v>103</v>
+      </c>
+      <c r="G30" s="25" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="31" ht="14.25" customHeight="1">
-      <c r="A31" s="23"/>
-      <c r="B31" s="22"/>
-      <c r="C31" s="23"/>
-      <c r="D31" s="23"/>
-      <c r="E31" s="23"/>
-      <c r="F31" s="23"/>
-      <c r="G31" s="23"/>
-    </row>
-    <row r="32" ht="14.25" customHeight="1"/>
-    <row r="33" ht="14.25" customHeight="1"/>
-    <row r="34" ht="14.25" customHeight="1"/>
-    <row r="35" ht="14.25" customHeight="1"/>
-    <row r="36" ht="14.25" customHeight="1"/>
+      <c r="A31" s="23">
+        <v>43890.0</v>
+      </c>
+      <c r="B31" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="C31" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="D31" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="E31" s="25" t="s">
+        <v>107</v>
+      </c>
+      <c r="F31" s="25" t="s">
+        <v>108</v>
+      </c>
+      <c r="G31" s="25" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="32" ht="14.25" customHeight="1">
+      <c r="A32" s="23">
+        <v>43894.0</v>
+      </c>
+      <c r="B32" s="24" t="s">
+        <v>110</v>
+      </c>
+      <c r="C32" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="D32" s="25" t="s">
+        <v>111</v>
+      </c>
+      <c r="E32" s="25" t="s">
+        <v>112</v>
+      </c>
+      <c r="F32" s="25" t="s">
+        <v>113</v>
+      </c>
+      <c r="G32" s="25" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="33" ht="14.25" customHeight="1">
+      <c r="A33" s="18"/>
+      <c r="B33" s="22"/>
+      <c r="C33" s="20"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="25"/>
+      <c r="G33" s="18"/>
+    </row>
+    <row r="34" ht="14.25" customHeight="1">
+      <c r="A34" s="18"/>
+      <c r="B34" s="22"/>
+      <c r="C34" s="20"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="25"/>
+      <c r="G34" s="18"/>
+    </row>
+    <row r="35" ht="14.25" customHeight="1">
+      <c r="A35" s="18"/>
+      <c r="B35" s="22"/>
+      <c r="C35" s="20"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="18"/>
+      <c r="F35" s="25"/>
+      <c r="G35" s="18"/>
+    </row>
+    <row r="36" ht="14.25" customHeight="1">
+      <c r="A36" s="18"/>
+      <c r="B36" s="22"/>
+      <c r="C36" s="20"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="18"/>
+      <c r="G36" s="18"/>
+    </row>
     <row r="37" ht="14.25" customHeight="1"/>
     <row r="38" ht="14.25" customHeight="1"/>
     <row r="39" ht="14.25" customHeight="1"/>

</xml_diff>